<commit_message>
added new annotation file
</commit_message>
<xml_diff>
--- a/anatomical-map/flatmap_annotation.xlsx
+++ b/anatomical-map/flatmap_annotation.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nebr002\work\sparc\flatmaps\rat\powerpoint\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nebr002\work\sparc\flatmaps-wip\rat\powerpoint\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Body organs" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1932" uniqueCount="1169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2016" uniqueCount="1228">
   <si>
     <t>Power point identifier</t>
   </si>
@@ -3531,6 +3531,183 @@
   </si>
   <si>
     <t xml:space="preserve">ILX:0734307 </t>
+  </si>
+  <si>
+    <t>digestive_34</t>
+  </si>
+  <si>
+    <t>digestive_35</t>
+  </si>
+  <si>
+    <t>digestive_36</t>
+  </si>
+  <si>
+    <t>digestive_37</t>
+  </si>
+  <si>
+    <t>digestive_38</t>
+  </si>
+  <si>
+    <t>digestive_39</t>
+  </si>
+  <si>
+    <t>digestive_40</t>
+  </si>
+  <si>
+    <t>digestive_41</t>
+  </si>
+  <si>
+    <t>digestive_42</t>
+  </si>
+  <si>
+    <t>serosa of small intestine</t>
+  </si>
+  <si>
+    <t>UBERON:0001206</t>
+  </si>
+  <si>
+    <t>UBERON:0001736</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILX:0727465 </t>
+  </si>
+  <si>
+    <t>small intestine smooth muscle longitudinal layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBERON:0012402 </t>
+  </si>
+  <si>
+    <t>ILX:0730357</t>
+  </si>
+  <si>
+    <t>myenteric nerve plexus</t>
+  </si>
+  <si>
+    <t>UBERON:0002439</t>
+  </si>
+  <si>
+    <t>ILX:0725342</t>
+  </si>
+  <si>
+    <t>small intestine smooth muscle circular layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBERON:0012401 </t>
+  </si>
+  <si>
+    <t>ILX:0736319</t>
+  </si>
+  <si>
+    <t>submucous nerve plexus</t>
+  </si>
+  <si>
+    <t>UBERON:0005304</t>
+  </si>
+  <si>
+    <t>ILX:0736047</t>
+  </si>
+  <si>
+    <t>lamina propria of small intestine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBERON:0001238 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILX:0736597  </t>
+  </si>
+  <si>
+    <t>epithelium of small intestine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBERON:0001902 </t>
+  </si>
+  <si>
+    <t>ILX:0730205</t>
+  </si>
+  <si>
+    <t>lumen of intestine</t>
+  </si>
+  <si>
+    <t>UBERON:0018543</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILX:0727722 </t>
+  </si>
+  <si>
+    <t>small intestine Peyer's patch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBERON:0003454  </t>
+  </si>
+  <si>
+    <t>ILX:0734825</t>
+  </si>
+  <si>
+    <t>mawe_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">superior mesenteric ganglion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBERON:0005479 </t>
+  </si>
+  <si>
+    <t>ILX:0732970</t>
+  </si>
+  <si>
+    <t>Sup.Mes.Gang</t>
+  </si>
+  <si>
+    <t>lumen</t>
+  </si>
+  <si>
+    <t>peyer's patch</t>
+  </si>
+  <si>
+    <t>lamina propria</t>
+  </si>
+  <si>
+    <t>submucosal plexus</t>
+  </si>
+  <si>
+    <t>CIRC M.</t>
+  </si>
+  <si>
+    <t>myenteric plexus</t>
+  </si>
+  <si>
+    <t>long M.</t>
+  </si>
+  <si>
+    <t>serosa</t>
+  </si>
+  <si>
+    <t>mawe_2</t>
+  </si>
+  <si>
+    <t>celiac ganglion</t>
+  </si>
+  <si>
+    <t>muscularis mucosae of small intestine</t>
+  </si>
+  <si>
+    <t>digestive_43</t>
+  </si>
+  <si>
+    <t>UBERON:0001210</t>
+  </si>
+  <si>
+    <t>ILX:0730247</t>
+  </si>
+  <si>
+    <t>circulatory_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBERON:0001981 </t>
+  </si>
+  <si>
+    <t>ILX:0101359</t>
   </si>
 </sst>
 </file>
@@ -3617,7 +3794,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -3839,11 +4016,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -3955,13 +4154,20 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4181,28 +4387,28 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB1067"/>
+  <dimension ref="A1:AB1077"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
-      <selection activeCell="A119" sqref="A119:XFD119"/>
+    <sheetView topLeftCell="A115" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
+      <selection activeCell="A144" sqref="A144"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.265625" customWidth="1"/>
     <col min="2" max="2" width="22.73046875" customWidth="1"/>
     <col min="3" max="3" width="39.265625" customWidth="1"/>
-    <col min="4" max="4" width="42.46484375" customWidth="1"/>
-    <col min="5" max="5" width="25.53125" customWidth="1"/>
+    <col min="4" max="4" width="42.3984375" customWidth="1"/>
+    <col min="5" max="5" width="25.59765625" customWidth="1"/>
     <col min="6" max="7" width="5.265625" customWidth="1"/>
-    <col min="8" max="8" width="42.46484375" customWidth="1"/>
+    <col min="8" max="8" width="42.3984375" customWidth="1"/>
     <col min="9" max="9" width="13.265625" customWidth="1"/>
     <col min="10" max="11" width="5.265625" customWidth="1"/>
-    <col min="12" max="12" width="15.53125" customWidth="1"/>
-    <col min="13" max="13" width="33.46484375" customWidth="1"/>
-    <col min="14" max="14" width="13.53125" customWidth="1"/>
+    <col min="12" max="12" width="15.59765625" customWidth="1"/>
+    <col min="13" max="13" width="33.3984375" customWidth="1"/>
+    <col min="14" max="14" width="13.59765625" customWidth="1"/>
     <col min="15" max="16" width="5.265625" customWidth="1"/>
-    <col min="17" max="17" width="88.53125" customWidth="1"/>
+    <col min="17" max="17" width="88.59765625" customWidth="1"/>
     <col min="18" max="18" width="122.265625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7035,7 +7241,7 @@
       <c r="B92" s="43" t="s">
         <v>1078</v>
       </c>
-      <c r="C92" s="59" t="s">
+      <c r="C92" s="76" t="s">
         <v>20</v>
       </c>
       <c r="D92" s="21" t="s">
@@ -7044,7 +7250,7 @@
       <c r="E92" s="43" t="s">
         <v>1078</v>
       </c>
-      <c r="G92" s="29"/>
+      <c r="G92" s="77"/>
       <c r="H92" s="21" t="s">
         <v>1077</v>
       </c>
@@ -7066,7 +7272,7 @@
       <c r="B93" s="43" t="s">
         <v>1064</v>
       </c>
-      <c r="C93" s="59" t="s">
+      <c r="C93" s="76" t="s">
         <v>20</v>
       </c>
       <c r="D93" s="21" t="s">
@@ -7075,7 +7281,7 @@
       <c r="E93" s="43" t="s">
         <v>1064</v>
       </c>
-      <c r="G93" s="29"/>
+      <c r="G93" s="77"/>
       <c r="H93" s="21" t="s">
         <v>1063</v>
       </c>
@@ -7097,7 +7303,7 @@
       <c r="B94" s="43" t="s">
         <v>1067</v>
       </c>
-      <c r="C94" s="59" t="s">
+      <c r="C94" s="76" t="s">
         <v>20</v>
       </c>
       <c r="D94" s="21" t="s">
@@ -7106,7 +7312,7 @@
       <c r="E94" s="43" t="s">
         <v>1067</v>
       </c>
-      <c r="G94" s="29"/>
+      <c r="G94" s="77"/>
       <c r="H94" s="21" t="s">
         <v>1065</v>
       </c>
@@ -7128,7 +7334,7 @@
       <c r="B95" s="43" t="s">
         <v>1070</v>
       </c>
-      <c r="C95" s="59" t="s">
+      <c r="C95" s="76" t="s">
         <v>20</v>
       </c>
       <c r="D95" s="66" t="s">
@@ -7137,7 +7343,7 @@
       <c r="E95" s="43" t="s">
         <v>1070</v>
       </c>
-      <c r="G95" s="29"/>
+      <c r="G95" s="77"/>
       <c r="H95" s="66" t="s">
         <v>1071</v>
       </c>
@@ -7157,12 +7363,12 @@
         <v>1081</v>
       </c>
       <c r="B96" s="35"/>
-      <c r="C96" s="59"/>
+      <c r="C96" s="76"/>
       <c r="D96" s="66" t="s">
         <v>1083</v>
       </c>
       <c r="E96" s="43"/>
-      <c r="G96" s="29"/>
+      <c r="G96" s="77"/>
       <c r="H96" s="66"/>
       <c r="I96" s="43"/>
       <c r="K96" s="29"/>
@@ -7178,12 +7384,12 @@
         <v>1082</v>
       </c>
       <c r="B97" s="35"/>
-      <c r="C97" s="59"/>
+      <c r="C97" s="76"/>
       <c r="D97" s="66" t="s">
         <v>1084</v>
       </c>
       <c r="E97" s="43"/>
-      <c r="G97" s="29"/>
+      <c r="G97" s="77"/>
       <c r="H97" s="66"/>
       <c r="I97" s="43"/>
       <c r="K97" s="29"/>
@@ -7201,14 +7407,14 @@
       <c r="B98" s="43" t="s">
         <v>1088</v>
       </c>
-      <c r="C98" s="59"/>
+      <c r="C98" s="76"/>
       <c r="D98" s="66" t="s">
         <v>1087</v>
       </c>
       <c r="E98" s="43" t="s">
         <v>1088</v>
       </c>
-      <c r="G98" s="29"/>
+      <c r="G98" s="77"/>
       <c r="H98" s="66" t="s">
         <v>1087</v>
       </c>
@@ -7230,14 +7436,14 @@
       <c r="B99" s="43" t="s">
         <v>1092</v>
       </c>
-      <c r="C99" s="59"/>
+      <c r="C99" s="76"/>
       <c r="D99" s="21" t="s">
         <v>1091</v>
       </c>
       <c r="E99" s="43" t="s">
         <v>1092</v>
       </c>
-      <c r="G99" s="29"/>
+      <c r="G99" s="77"/>
       <c r="H99" s="21" t="s">
         <v>1091</v>
       </c>
@@ -7259,14 +7465,14 @@
       <c r="B100" s="43" t="s">
         <v>1109</v>
       </c>
-      <c r="C100" s="59"/>
+      <c r="C100" s="76"/>
       <c r="D100" s="66" t="s">
         <v>1108</v>
       </c>
       <c r="E100" s="43" t="s">
         <v>1109</v>
       </c>
-      <c r="G100" s="29"/>
+      <c r="G100" s="77"/>
       <c r="H100" s="66" t="s">
         <v>1108</v>
       </c>
@@ -7288,14 +7494,14 @@
       <c r="B101" s="43" t="s">
         <v>1102</v>
       </c>
-      <c r="C101" s="59"/>
+      <c r="C101" s="76"/>
       <c r="D101" s="66" t="s">
         <v>1101</v>
       </c>
       <c r="E101" s="43" t="s">
         <v>1102</v>
       </c>
-      <c r="G101" s="29"/>
+      <c r="G101" s="77"/>
       <c r="H101" s="66" t="s">
         <v>1112</v>
       </c>
@@ -7317,7 +7523,7 @@
       <c r="B102" s="68" t="s">
         <v>1121</v>
       </c>
-      <c r="C102" s="71" t="s">
+      <c r="C102" s="75" t="s">
         <v>1119</v>
       </c>
       <c r="D102" s="66" t="s">
@@ -7326,7 +7532,7 @@
       <c r="E102" s="68" t="s">
         <v>1121</v>
       </c>
-      <c r="G102" s="29"/>
+      <c r="G102" s="77"/>
       <c r="H102" s="66" t="s">
         <v>1120</v>
       </c>
@@ -7348,14 +7554,14 @@
       <c r="B103" s="68" t="s">
         <v>821</v>
       </c>
-      <c r="C103" s="59"/>
+      <c r="C103" s="76"/>
       <c r="D103" s="66" t="s">
         <v>820</v>
       </c>
       <c r="E103" s="68" t="s">
         <v>821</v>
       </c>
-      <c r="G103" s="29"/>
+      <c r="G103" s="77"/>
       <c r="H103" s="66" t="s">
         <v>820</v>
       </c>
@@ -7377,7 +7583,7 @@
       <c r="B104" s="68" t="s">
         <v>1127</v>
       </c>
-      <c r="C104" s="71" t="s">
+      <c r="C104" s="75" t="s">
         <v>1125</v>
       </c>
       <c r="D104" s="66" t="s">
@@ -7386,7 +7592,7 @@
       <c r="E104" s="68" t="s">
         <v>1127</v>
       </c>
-      <c r="G104" s="29"/>
+      <c r="G104" s="77"/>
       <c r="H104" s="66" t="s">
         <v>1126</v>
       </c>
@@ -7408,14 +7614,14 @@
       <c r="B105" s="68" t="s">
         <v>1146</v>
       </c>
-      <c r="C105" s="71"/>
+      <c r="C105" s="75"/>
       <c r="D105" s="66" t="s">
         <v>1147</v>
       </c>
       <c r="E105" s="68" t="s">
         <v>1146</v>
       </c>
-      <c r="G105" s="29"/>
+      <c r="G105" s="77"/>
       <c r="H105" s="66" t="s">
         <v>1147</v>
       </c>
@@ -7437,14 +7643,14 @@
       <c r="B106" s="65" t="s">
         <v>1151</v>
       </c>
-      <c r="C106" s="71"/>
+      <c r="C106" s="75"/>
       <c r="D106" s="66" t="s">
         <v>1150</v>
       </c>
       <c r="E106" s="68" t="s">
         <v>1151</v>
       </c>
-      <c r="G106" s="29"/>
+      <c r="G106" s="77"/>
       <c r="H106" s="66" t="s">
         <v>1150</v>
       </c>
@@ -7466,14 +7672,14 @@
       <c r="B107" s="65" t="s">
         <v>1159</v>
       </c>
-      <c r="C107" s="71"/>
+      <c r="C107" s="75"/>
       <c r="D107" s="66" t="s">
         <v>1157</v>
       </c>
       <c r="E107" s="68" t="s">
-        <v>1159</v>
-      </c>
-      <c r="G107" s="29"/>
+        <v>1180</v>
+      </c>
+      <c r="G107" s="77"/>
       <c r="H107" s="66" t="s">
         <v>1157</v>
       </c>
@@ -7489,13 +7695,28 @@
       <c r="R107" s="40"/>
     </row>
     <row r="108" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A108" s="27"/>
-      <c r="B108" s="39"/>
-      <c r="D108" s="31"/>
-      <c r="E108" s="33"/>
-      <c r="G108" s="29"/>
-      <c r="H108" s="31"/>
-      <c r="I108" s="33"/>
+      <c r="A108" s="35" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B108" s="65" t="s">
+        <v>1179</v>
+      </c>
+      <c r="C108" s="75" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D108" s="66" t="s">
+        <v>1178</v>
+      </c>
+      <c r="E108" s="68" t="s">
+        <v>1179</v>
+      </c>
+      <c r="G108" s="77"/>
+      <c r="H108" s="66" t="s">
+        <v>1178</v>
+      </c>
+      <c r="I108" s="68" t="s">
+        <v>1181</v>
+      </c>
       <c r="K108" s="29"/>
       <c r="L108" s="31"/>
       <c r="M108" s="29"/>
@@ -7505,27 +7726,27 @@
       <c r="R108" s="40"/>
     </row>
     <row r="109" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A109" s="19" t="s">
-        <v>833</v>
-      </c>
-      <c r="B109" s="43" t="s">
-        <v>835</v>
-      </c>
-      <c r="C109" s="21" t="s">
-        <v>834</v>
-      </c>
-      <c r="D109" s="23" t="s">
-        <v>834</v>
-      </c>
-      <c r="E109" s="26" t="s">
-        <v>835</v>
-      </c>
-      <c r="G109" s="29"/>
-      <c r="H109" s="23" t="s">
-        <v>834</v>
-      </c>
-      <c r="I109" s="26" t="s">
-        <v>836</v>
+      <c r="A109" s="35" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B109" s="65" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C109" s="75" t="s">
+        <v>1217</v>
+      </c>
+      <c r="D109" s="66" t="s">
+        <v>1182</v>
+      </c>
+      <c r="E109" s="68" t="s">
+        <v>1183</v>
+      </c>
+      <c r="G109" s="77"/>
+      <c r="H109" s="66" t="s">
+        <v>1182</v>
+      </c>
+      <c r="I109" s="68" t="s">
+        <v>1184</v>
       </c>
       <c r="K109" s="29"/>
       <c r="L109" s="31"/>
@@ -7533,32 +7754,30 @@
       <c r="N109" s="33"/>
       <c r="P109" s="29"/>
       <c r="Q109" s="32"/>
-      <c r="R109" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R109" s="40"/>
     </row>
     <row r="110" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A110" s="65" t="s">
-        <v>837</v>
-      </c>
-      <c r="B110" s="43" t="s">
-        <v>839</v>
-      </c>
-      <c r="C110" s="21" t="s">
-        <v>838</v>
-      </c>
-      <c r="D110" s="23" t="s">
-        <v>838</v>
-      </c>
-      <c r="E110" s="26" t="s">
-        <v>839</v>
-      </c>
-      <c r="G110" s="29"/>
-      <c r="H110" s="23" t="s">
-        <v>838</v>
-      </c>
-      <c r="I110" s="26" t="s">
-        <v>840</v>
+      <c r="A110" s="35" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B110" s="65" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C110" s="75" t="s">
+        <v>1216</v>
+      </c>
+      <c r="D110" s="66" t="s">
+        <v>1185</v>
+      </c>
+      <c r="E110" s="68" t="s">
+        <v>1186</v>
+      </c>
+      <c r="G110" s="77"/>
+      <c r="H110" s="66" t="s">
+        <v>1185</v>
+      </c>
+      <c r="I110" s="68" t="s">
+        <v>1187</v>
       </c>
       <c r="K110" s="29"/>
       <c r="L110" s="31"/>
@@ -7566,32 +7785,30 @@
       <c r="N110" s="33"/>
       <c r="P110" s="29"/>
       <c r="Q110" s="32"/>
-      <c r="R110" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R110" s="40"/>
     </row>
     <row r="111" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A111" s="19" t="s">
-        <v>841</v>
-      </c>
-      <c r="B111" s="43" t="s">
-        <v>843</v>
-      </c>
-      <c r="C111" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D111" s="23" t="s">
-        <v>842</v>
-      </c>
-      <c r="E111" s="26" t="s">
-        <v>843</v>
-      </c>
-      <c r="G111" s="29"/>
-      <c r="H111" s="42" t="s">
-        <v>842</v>
-      </c>
-      <c r="I111" s="26" t="s">
-        <v>844</v>
+      <c r="A111" s="35" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B111" s="65" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C111" s="75" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D111" s="66" t="s">
+        <v>1188</v>
+      </c>
+      <c r="E111" s="68" t="s">
+        <v>1189</v>
+      </c>
+      <c r="G111" s="77"/>
+      <c r="H111" s="66" t="s">
+        <v>1188</v>
+      </c>
+      <c r="I111" s="68" t="s">
+        <v>1190</v>
       </c>
       <c r="K111" s="29"/>
       <c r="L111" s="31"/>
@@ -7599,32 +7816,30 @@
       <c r="N111" s="33"/>
       <c r="P111" s="29"/>
       <c r="Q111" s="32"/>
-      <c r="R111" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R111" s="40"/>
     </row>
     <row r="112" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A112" s="19" t="s">
-        <v>845</v>
-      </c>
-      <c r="B112" s="43" t="s">
-        <v>847</v>
-      </c>
-      <c r="C112" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D112" s="23" t="s">
-        <v>846</v>
-      </c>
-      <c r="E112" s="26" t="s">
-        <v>847</v>
-      </c>
-      <c r="G112" s="29"/>
-      <c r="H112" s="42" t="s">
-        <v>846</v>
-      </c>
-      <c r="I112" s="26" t="s">
-        <v>848</v>
+      <c r="A112" s="35" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B112" s="65" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C112" s="75" t="s">
+        <v>1214</v>
+      </c>
+      <c r="D112" s="66" t="s">
+        <v>1191</v>
+      </c>
+      <c r="E112" s="68" t="s">
+        <v>1192</v>
+      </c>
+      <c r="G112" s="77"/>
+      <c r="H112" s="66" t="s">
+        <v>1191</v>
+      </c>
+      <c r="I112" s="68" t="s">
+        <v>1193</v>
       </c>
       <c r="K112" s="29"/>
       <c r="L112" s="31"/>
@@ -7632,32 +7847,30 @@
       <c r="N112" s="33"/>
       <c r="P112" s="29"/>
       <c r="Q112" s="32"/>
-      <c r="R112" s="34" t="s">
-        <v>849</v>
-      </c>
+      <c r="R112" s="40"/>
     </row>
     <row r="113" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A113" s="19" t="s">
-        <v>850</v>
-      </c>
-      <c r="B113" s="43" t="s">
-        <v>852</v>
-      </c>
-      <c r="C113" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D113" s="23" t="s">
-        <v>851</v>
-      </c>
-      <c r="E113" s="26" t="s">
-        <v>852</v>
-      </c>
-      <c r="G113" s="29"/>
-      <c r="H113" s="42" t="s">
-        <v>851</v>
-      </c>
-      <c r="I113" s="26" t="s">
-        <v>853</v>
+      <c r="A113" s="35" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B113" s="65" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C113" s="75" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D113" s="66" t="s">
+        <v>1194</v>
+      </c>
+      <c r="E113" s="68" t="s">
+        <v>1195</v>
+      </c>
+      <c r="G113" s="77"/>
+      <c r="H113" s="66" t="s">
+        <v>1194</v>
+      </c>
+      <c r="I113" s="68" t="s">
+        <v>1196</v>
       </c>
       <c r="K113" s="29"/>
       <c r="L113" s="31"/>
@@ -7665,30 +7878,30 @@
       <c r="N113" s="33"/>
       <c r="P113" s="29"/>
       <c r="Q113" s="32"/>
-      <c r="R113" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R113" s="40"/>
     </row>
     <row r="114" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A114" s="35" t="s">
-        <v>1093</v>
-      </c>
-      <c r="B114" s="68" t="s">
-        <v>1113</v>
-      </c>
-      <c r="C114" s="21"/>
-      <c r="D114" s="67" t="s">
-        <v>1094</v>
+        <v>1175</v>
+      </c>
+      <c r="B114" s="65" t="s">
+        <v>1198</v>
+      </c>
+      <c r="C114" s="75" t="s">
+        <v>203</v>
+      </c>
+      <c r="D114" s="66" t="s">
+        <v>1197</v>
       </c>
       <c r="E114" s="68" t="s">
-        <v>1113</v>
-      </c>
-      <c r="G114" s="29"/>
-      <c r="H114" s="67" t="s">
-        <v>1094</v>
-      </c>
-      <c r="I114" s="43" t="s">
-        <v>1114</v>
+        <v>1198</v>
+      </c>
+      <c r="G114" s="77"/>
+      <c r="H114" s="66" t="s">
+        <v>1197</v>
+      </c>
+      <c r="I114" s="68" t="s">
+        <v>1199</v>
       </c>
       <c r="K114" s="29"/>
       <c r="L114" s="31"/>
@@ -7700,24 +7913,26 @@
     </row>
     <row r="115" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A115" s="35" t="s">
-        <v>1096</v>
-      </c>
-      <c r="B115" s="43" t="s">
-        <v>1098</v>
-      </c>
-      <c r="C115" s="21"/>
-      <c r="D115" s="42" t="s">
-        <v>1097</v>
-      </c>
-      <c r="E115" s="43" t="s">
-        <v>1098</v>
-      </c>
-      <c r="G115" s="29"/>
-      <c r="H115" s="42" t="s">
-        <v>1097</v>
-      </c>
-      <c r="I115" s="43" t="s">
-        <v>1099</v>
+        <v>1176</v>
+      </c>
+      <c r="B115" s="65" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C115" s="75" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D115" s="66" t="s">
+        <v>1200</v>
+      </c>
+      <c r="E115" s="68" t="s">
+        <v>1201</v>
+      </c>
+      <c r="G115" s="77"/>
+      <c r="H115" s="66" t="s">
+        <v>1200</v>
+      </c>
+      <c r="I115" s="68" t="s">
+        <v>1202</v>
       </c>
       <c r="K115" s="29"/>
       <c r="L115" s="31"/>
@@ -7729,24 +7944,26 @@
     </row>
     <row r="116" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A116" s="35" t="s">
-        <v>1153</v>
-      </c>
-      <c r="B116" s="35" t="s">
-        <v>1154</v>
-      </c>
-      <c r="C116" s="21"/>
-      <c r="D116" s="67" t="s">
-        <v>1155</v>
-      </c>
-      <c r="E116" s="35" t="s">
-        <v>1154</v>
-      </c>
-      <c r="G116" s="29"/>
-      <c r="H116" s="42" t="s">
-        <v>1155</v>
-      </c>
-      <c r="I116" s="43" t="s">
-        <v>1156</v>
+        <v>1177</v>
+      </c>
+      <c r="B116" s="65" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C116" s="75" t="s">
+        <v>1212</v>
+      </c>
+      <c r="D116" s="74" t="s">
+        <v>1203</v>
+      </c>
+      <c r="E116" s="68" t="s">
+        <v>1204</v>
+      </c>
+      <c r="G116" s="77"/>
+      <c r="H116" s="66" t="s">
+        <v>1203</v>
+      </c>
+      <c r="I116" s="68" t="s">
+        <v>1205</v>
       </c>
       <c r="K116" s="29"/>
       <c r="L116" s="31"/>
@@ -7757,73 +7974,72 @@
       <c r="R116" s="40"/>
     </row>
     <row r="117" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A117" s="27"/>
-      <c r="B117" s="39"/>
-      <c r="D117" s="31"/>
-      <c r="E117" s="33"/>
+      <c r="A117" s="35" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B117" s="65" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C117" s="78"/>
+      <c r="D117" s="78" t="s">
+        <v>1221</v>
+      </c>
+      <c r="E117" s="68" t="s">
+        <v>1223</v>
+      </c>
       <c r="G117" s="29"/>
-      <c r="H117" s="31"/>
-      <c r="I117" s="33"/>
+      <c r="H117" s="66" t="s">
+        <v>1221</v>
+      </c>
+      <c r="I117" s="68" t="s">
+        <v>1224</v>
+      </c>
       <c r="K117" s="29"/>
       <c r="L117" s="31"/>
       <c r="M117" s="29"/>
       <c r="N117" s="33"/>
       <c r="P117" s="29"/>
       <c r="Q117" s="32"/>
-      <c r="R117" s="34"/>
+      <c r="R117" s="40"/>
     </row>
     <row r="118" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A118" s="19" t="s">
-        <v>854</v>
-      </c>
-      <c r="B118" s="43" t="s">
-        <v>857</v>
-      </c>
-      <c r="C118" s="21" t="s">
-        <v>855</v>
-      </c>
-      <c r="D118" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E118" s="26" t="s">
-        <v>20</v>
-      </c>
+      <c r="A118" s="27"/>
+      <c r="B118" s="39"/>
+      <c r="D118" s="31"/>
+      <c r="E118" s="33"/>
       <c r="G118" s="29"/>
-      <c r="H118" s="23" t="s">
-        <v>856</v>
-      </c>
-      <c r="I118" s="26" t="s">
-        <v>857</v>
-      </c>
+      <c r="H118" s="31"/>
+      <c r="I118" s="33"/>
       <c r="K118" s="29"/>
       <c r="L118" s="31"/>
       <c r="M118" s="29"/>
       <c r="N118" s="33"/>
       <c r="P118" s="29"/>
       <c r="Q118" s="32"/>
-      <c r="R118" s="34" t="s">
-        <v>849</v>
-      </c>
+      <c r="R118" s="40"/>
     </row>
     <row r="119" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A119" s="35" t="s">
-        <v>1165</v>
-      </c>
-      <c r="B119" s="33" t="s">
-        <v>1166</v>
-      </c>
-      <c r="D119" s="70" t="s">
-        <v>1167</v>
-      </c>
-      <c r="E119" s="33" t="s">
-        <v>1166</v>
+      <c r="A119" s="19" t="s">
+        <v>833</v>
+      </c>
+      <c r="B119" s="43" t="s">
+        <v>835</v>
+      </c>
+      <c r="C119" s="21" t="s">
+        <v>834</v>
+      </c>
+      <c r="D119" s="23" t="s">
+        <v>834</v>
+      </c>
+      <c r="E119" s="26" t="s">
+        <v>835</v>
       </c>
       <c r="G119" s="29"/>
-      <c r="H119" s="70" t="s">
-        <v>1167</v>
-      </c>
-      <c r="I119" s="33" t="s">
-        <v>1168</v>
+      <c r="H119" s="23" t="s">
+        <v>834</v>
+      </c>
+      <c r="I119" s="26" t="s">
+        <v>836</v>
       </c>
       <c r="K119" s="29"/>
       <c r="L119" s="31"/>
@@ -7831,47 +8047,65 @@
       <c r="N119" s="33"/>
       <c r="P119" s="29"/>
       <c r="Q119" s="32"/>
-      <c r="R119" s="40"/>
+      <c r="R119" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="120" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A120" s="19"/>
-      <c r="B120" s="39"/>
-      <c r="C120" s="21"/>
-      <c r="D120" s="31"/>
-      <c r="E120" s="33"/>
+      <c r="A120" s="65" t="s">
+        <v>837</v>
+      </c>
+      <c r="B120" s="43" t="s">
+        <v>839</v>
+      </c>
+      <c r="C120" s="21" t="s">
+        <v>838</v>
+      </c>
+      <c r="D120" s="23" t="s">
+        <v>838</v>
+      </c>
+      <c r="E120" s="26" t="s">
+        <v>839</v>
+      </c>
       <c r="G120" s="29"/>
-      <c r="H120" s="31"/>
-      <c r="I120" s="33"/>
+      <c r="H120" s="23" t="s">
+        <v>838</v>
+      </c>
+      <c r="I120" s="26" t="s">
+        <v>840</v>
+      </c>
       <c r="K120" s="29"/>
       <c r="L120" s="31"/>
       <c r="M120" s="29"/>
       <c r="N120" s="33"/>
       <c r="P120" s="29"/>
       <c r="Q120" s="32"/>
-      <c r="R120" s="40"/>
+      <c r="R120" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="121" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A121" s="65" t="s">
-        <v>858</v>
+      <c r="A121" s="19" t="s">
+        <v>841</v>
       </c>
       <c r="B121" s="43" t="s">
-        <v>860</v>
-      </c>
-      <c r="C121" s="19" t="s">
-        <v>859</v>
-      </c>
-      <c r="D121" s="21" t="s">
-        <v>859</v>
+        <v>843</v>
+      </c>
+      <c r="C121" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D121" s="23" t="s">
+        <v>842</v>
       </c>
       <c r="E121" s="26" t="s">
-        <v>860</v>
-      </c>
-      <c r="G121" s="33"/>
-      <c r="H121" s="21" t="s">
-        <v>859</v>
+        <v>843</v>
+      </c>
+      <c r="G121" s="29"/>
+      <c r="H121" s="42" t="s">
+        <v>842</v>
       </c>
       <c r="I121" s="26" t="s">
-        <v>861</v>
+        <v>844</v>
       </c>
       <c r="K121" s="29"/>
       <c r="L121" s="31"/>
@@ -7885,26 +8119,26 @@
     </row>
     <row r="122" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A122" s="19" t="s">
-        <v>862</v>
+        <v>845</v>
       </c>
       <c r="B122" s="43" t="s">
-        <v>864</v>
+        <v>847</v>
       </c>
       <c r="C122" s="21" t="s">
-        <v>863</v>
+        <v>20</v>
       </c>
       <c r="D122" s="23" t="s">
-        <v>863</v>
+        <v>846</v>
       </c>
       <c r="E122" s="26" t="s">
-        <v>864</v>
+        <v>847</v>
       </c>
       <c r="G122" s="29"/>
-      <c r="H122" s="23" t="s">
-        <v>863</v>
+      <c r="H122" s="42" t="s">
+        <v>846</v>
       </c>
       <c r="I122" s="26" t="s">
-        <v>865</v>
+        <v>848</v>
       </c>
       <c r="K122" s="29"/>
       <c r="L122" s="31"/>
@@ -7912,30 +8146,32 @@
       <c r="N122" s="33"/>
       <c r="P122" s="29"/>
       <c r="Q122" s="32"/>
-      <c r="R122" s="34" t="b">
-        <v>1</v>
+      <c r="R122" s="34" t="s">
+        <v>849</v>
       </c>
     </row>
     <row r="123" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A123" s="65" t="s">
-        <v>1145</v>
-      </c>
-      <c r="B123" s="68" t="s">
-        <v>1143</v>
-      </c>
-      <c r="C123" s="71"/>
-      <c r="D123" s="66" t="s">
-        <v>1142</v>
-      </c>
-      <c r="E123" s="68" t="s">
-        <v>1143</v>
+      <c r="A123" s="19" t="s">
+        <v>850</v>
+      </c>
+      <c r="B123" s="43" t="s">
+        <v>852</v>
+      </c>
+      <c r="C123" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D123" s="23" t="s">
+        <v>851</v>
+      </c>
+      <c r="E123" s="26" t="s">
+        <v>852</v>
       </c>
       <c r="G123" s="29"/>
-      <c r="H123" s="66" t="s">
-        <v>1142</v>
-      </c>
-      <c r="I123" s="68" t="s">
-        <v>1144</v>
+      <c r="H123" s="42" t="s">
+        <v>851</v>
+      </c>
+      <c r="I123" s="26" t="s">
+        <v>853</v>
       </c>
       <c r="K123" s="29"/>
       <c r="L123" s="31"/>
@@ -7943,16 +8179,31 @@
       <c r="N123" s="33"/>
       <c r="P123" s="29"/>
       <c r="Q123" s="32"/>
-      <c r="R123" s="40"/>
+      <c r="R123" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="124" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A124" s="27"/>
-      <c r="B124" s="39"/>
-      <c r="D124" s="31"/>
-      <c r="E124" s="33"/>
+      <c r="A124" s="35" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B124" s="68" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C124" s="21"/>
+      <c r="D124" s="67" t="s">
+        <v>1094</v>
+      </c>
+      <c r="E124" s="68" t="s">
+        <v>1113</v>
+      </c>
       <c r="G124" s="29"/>
-      <c r="H124" s="31"/>
-      <c r="I124" s="33"/>
+      <c r="H124" s="67" t="s">
+        <v>1094</v>
+      </c>
+      <c r="I124" s="43" t="s">
+        <v>1114</v>
+      </c>
       <c r="K124" s="29"/>
       <c r="L124" s="31"/>
       <c r="M124" s="29"/>
@@ -7962,27 +8213,25 @@
       <c r="R124" s="40"/>
     </row>
     <row r="125" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A125" s="19" t="s">
-        <v>866</v>
+      <c r="A125" s="35" t="s">
+        <v>1096</v>
       </c>
       <c r="B125" s="43" t="s">
-        <v>868</v>
-      </c>
-      <c r="C125" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D125" s="23" t="s">
-        <v>867</v>
-      </c>
-      <c r="E125" s="26" t="s">
-        <v>868</v>
+        <v>1098</v>
+      </c>
+      <c r="C125" s="21"/>
+      <c r="D125" s="42" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E125" s="43" t="s">
+        <v>1098</v>
       </c>
       <c r="G125" s="29"/>
-      <c r="H125" s="23" t="s">
-        <v>867</v>
-      </c>
-      <c r="I125" s="26" t="s">
-        <v>869</v>
+      <c r="H125" s="42" t="s">
+        <v>1097</v>
+      </c>
+      <c r="I125" s="43" t="s">
+        <v>1099</v>
       </c>
       <c r="K125" s="29"/>
       <c r="L125" s="31"/>
@@ -7990,32 +8239,28 @@
       <c r="N125" s="33"/>
       <c r="P125" s="29"/>
       <c r="Q125" s="32"/>
-      <c r="R125" s="34" t="s">
-        <v>33</v>
-      </c>
+      <c r="R125" s="40"/>
     </row>
     <row r="126" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A126" s="19" t="s">
-        <v>870</v>
-      </c>
-      <c r="B126" s="43" t="s">
-        <v>872</v>
-      </c>
-      <c r="C126" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D126" s="23" t="s">
-        <v>871</v>
-      </c>
-      <c r="E126" s="26" t="s">
-        <v>872</v>
+      <c r="A126" s="35" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B126" s="35" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C126" s="21"/>
+      <c r="D126" s="67" t="s">
+        <v>1155</v>
+      </c>
+      <c r="E126" s="35" t="s">
+        <v>1154</v>
       </c>
       <c r="G126" s="29"/>
-      <c r="H126" s="23" t="s">
-        <v>871</v>
-      </c>
-      <c r="I126" s="26" t="s">
-        <v>873</v>
+      <c r="H126" s="42" t="s">
+        <v>1155</v>
+      </c>
+      <c r="I126" s="43" t="s">
+        <v>1156</v>
       </c>
       <c r="K126" s="29"/>
       <c r="L126" s="31"/>
@@ -8023,65 +8268,46 @@
       <c r="N126" s="33"/>
       <c r="P126" s="29"/>
       <c r="Q126" s="32"/>
-      <c r="R126" s="34" t="s">
-        <v>33</v>
-      </c>
+      <c r="R126" s="40"/>
     </row>
     <row r="127" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A127" s="19" t="s">
-        <v>874</v>
-      </c>
-      <c r="B127" s="43" t="s">
-        <v>876</v>
-      </c>
-      <c r="C127" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D127" s="23" t="s">
-        <v>875</v>
-      </c>
-      <c r="E127" s="26" t="s">
-        <v>876</v>
-      </c>
+      <c r="A127" s="27"/>
+      <c r="B127" s="39"/>
+      <c r="D127" s="31"/>
+      <c r="E127" s="33"/>
       <c r="G127" s="29"/>
-      <c r="H127" s="23" t="s">
-        <v>875</v>
-      </c>
-      <c r="I127" s="26" t="s">
-        <v>877</v>
-      </c>
+      <c r="H127" s="31"/>
+      <c r="I127" s="33"/>
       <c r="K127" s="29"/>
       <c r="L127" s="31"/>
       <c r="M127" s="29"/>
       <c r="N127" s="33"/>
       <c r="P127" s="29"/>
       <c r="Q127" s="32"/>
-      <c r="R127" s="34" t="s">
-        <v>33</v>
-      </c>
+      <c r="R127" s="34"/>
     </row>
     <row r="128" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A128" s="19" t="s">
-        <v>878</v>
+        <v>854</v>
       </c>
       <c r="B128" s="43" t="s">
-        <v>880</v>
+        <v>857</v>
       </c>
       <c r="C128" s="21" t="s">
+        <v>855</v>
+      </c>
+      <c r="D128" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="D128" s="23" t="s">
-        <v>879</v>
-      </c>
       <c r="E128" s="26" t="s">
-        <v>880</v>
+        <v>20</v>
       </c>
       <c r="G128" s="29"/>
       <c r="H128" s="23" t="s">
-        <v>879</v>
+        <v>856</v>
       </c>
       <c r="I128" s="26" t="s">
-        <v>881</v>
+        <v>857</v>
       </c>
       <c r="K128" s="29"/>
       <c r="L128" s="31"/>
@@ -8089,32 +8315,29 @@
       <c r="N128" s="33"/>
       <c r="P128" s="29"/>
       <c r="Q128" s="32"/>
-      <c r="R128" s="34" t="b">
-        <v>1</v>
+      <c r="R128" s="34" t="s">
+        <v>849</v>
       </c>
     </row>
     <row r="129" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A129" s="19" t="s">
-        <v>882</v>
-      </c>
-      <c r="B129" s="43" t="s">
-        <v>884</v>
-      </c>
-      <c r="C129" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D129" s="23" t="s">
-        <v>883</v>
-      </c>
-      <c r="E129" s="26" t="s">
-        <v>884</v>
+      <c r="A129" s="35" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B129" s="33" t="s">
+        <v>1166</v>
+      </c>
+      <c r="D129" s="70" t="s">
+        <v>1167</v>
+      </c>
+      <c r="E129" s="33" t="s">
+        <v>1166</v>
       </c>
       <c r="G129" s="29"/>
-      <c r="H129" s="23" t="s">
-        <v>883</v>
-      </c>
-      <c r="I129" s="26" t="s">
-        <v>885</v>
+      <c r="H129" s="70" t="s">
+        <v>1167</v>
+      </c>
+      <c r="I129" s="33" t="s">
+        <v>1168</v>
       </c>
       <c r="K129" s="29"/>
       <c r="L129" s="31"/>
@@ -8122,65 +8345,47 @@
       <c r="N129" s="33"/>
       <c r="P129" s="29"/>
       <c r="Q129" s="32"/>
-      <c r="R129" s="34" t="s">
-        <v>33</v>
-      </c>
+      <c r="R129" s="40"/>
     </row>
     <row r="130" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A130" s="19" t="s">
-        <v>886</v>
-      </c>
-      <c r="B130" s="43" t="s">
-        <v>888</v>
-      </c>
-      <c r="C130" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D130" s="23" t="s">
-        <v>887</v>
-      </c>
-      <c r="E130" s="26" t="s">
-        <v>888</v>
-      </c>
+      <c r="A130" s="19"/>
+      <c r="B130" s="39"/>
+      <c r="C130" s="21"/>
+      <c r="D130" s="31"/>
+      <c r="E130" s="33"/>
       <c r="G130" s="29"/>
-      <c r="H130" s="23" t="s">
-        <v>887</v>
-      </c>
-      <c r="I130" s="26" t="s">
-        <v>889</v>
-      </c>
+      <c r="H130" s="31"/>
+      <c r="I130" s="33"/>
       <c r="K130" s="29"/>
       <c r="L130" s="31"/>
       <c r="M130" s="29"/>
       <c r="N130" s="33"/>
       <c r="P130" s="29"/>
       <c r="Q130" s="32"/>
-      <c r="R130" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R130" s="40"/>
     </row>
     <row r="131" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A131" s="19" t="s">
-        <v>890</v>
+      <c r="A131" s="65" t="s">
+        <v>858</v>
       </c>
       <c r="B131" s="43" t="s">
-        <v>892</v>
-      </c>
-      <c r="C131" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D131" s="23" t="s">
-        <v>891</v>
+        <v>860</v>
+      </c>
+      <c r="C131" s="19" t="s">
+        <v>859</v>
+      </c>
+      <c r="D131" s="21" t="s">
+        <v>859</v>
       </c>
       <c r="E131" s="26" t="s">
-        <v>892</v>
-      </c>
-      <c r="G131" s="29"/>
-      <c r="H131" s="23" t="s">
-        <v>891</v>
+        <v>860</v>
+      </c>
+      <c r="G131" s="33"/>
+      <c r="H131" s="21" t="s">
+        <v>859</v>
       </c>
       <c r="I131" s="26" t="s">
-        <v>893</v>
+        <v>861</v>
       </c>
       <c r="K131" s="29"/>
       <c r="L131" s="31"/>
@@ -8193,24 +8398,27 @@
       </c>
     </row>
     <row r="132" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A132" s="27" t="s">
-        <v>1072</v>
-      </c>
-      <c r="B132" s="69" t="s">
-        <v>1115</v>
-      </c>
-      <c r="D132" s="70" t="s">
-        <v>1073</v>
-      </c>
-      <c r="E132" s="69" t="s">
-        <v>1115</v>
+      <c r="A132" s="19" t="s">
+        <v>862</v>
+      </c>
+      <c r="B132" s="43" t="s">
+        <v>864</v>
+      </c>
+      <c r="C132" s="21" t="s">
+        <v>863</v>
+      </c>
+      <c r="D132" s="23" t="s">
+        <v>863</v>
+      </c>
+      <c r="E132" s="26" t="s">
+        <v>864</v>
       </c>
       <c r="G132" s="29"/>
-      <c r="H132" s="70" t="s">
-        <v>1073</v>
-      </c>
-      <c r="I132" s="69" t="s">
-        <v>1116</v>
+      <c r="H132" s="23" t="s">
+        <v>863</v>
+      </c>
+      <c r="I132" s="26" t="s">
+        <v>865</v>
       </c>
       <c r="K132" s="29"/>
       <c r="L132" s="31"/>
@@ -8218,23 +8426,38 @@
       <c r="N132" s="33"/>
       <c r="P132" s="29"/>
       <c r="Q132" s="32"/>
-      <c r="R132" s="27"/>
+      <c r="R132" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="133" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A133" s="27"/>
-      <c r="B133" s="39"/>
-      <c r="D133" s="31"/>
-      <c r="E133" s="33"/>
-      <c r="G133" s="29"/>
-      <c r="H133" s="31"/>
-      <c r="I133" s="33"/>
+      <c r="A133" s="65" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B133" s="68" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C133" s="75"/>
+      <c r="D133" s="66" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E133" s="68" t="s">
+        <v>1143</v>
+      </c>
+      <c r="G133" s="77"/>
+      <c r="H133" s="66" t="s">
+        <v>1142</v>
+      </c>
+      <c r="I133" s="68" t="s">
+        <v>1144</v>
+      </c>
       <c r="K133" s="29"/>
       <c r="L133" s="31"/>
       <c r="M133" s="29"/>
       <c r="N133" s="33"/>
       <c r="P133" s="29"/>
       <c r="Q133" s="32"/>
-      <c r="R133" s="27"/>
+      <c r="R133" s="40"/>
     </row>
     <row r="134" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A134" s="27"/>
@@ -8250,128 +8473,259 @@
       <c r="N134" s="33"/>
       <c r="P134" s="29"/>
       <c r="Q134" s="32"/>
-      <c r="R134" s="27"/>
+      <c r="R134" s="40"/>
     </row>
     <row r="135" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A135" s="27"/>
-      <c r="B135" s="39"/>
-      <c r="D135" s="31"/>
-      <c r="E135" s="33"/>
+      <c r="A135" s="19" t="s">
+        <v>866</v>
+      </c>
+      <c r="B135" s="43" t="s">
+        <v>868</v>
+      </c>
+      <c r="C135" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D135" s="23" t="s">
+        <v>867</v>
+      </c>
+      <c r="E135" s="26" t="s">
+        <v>868</v>
+      </c>
       <c r="G135" s="29"/>
-      <c r="H135" s="31"/>
-      <c r="I135" s="33"/>
+      <c r="H135" s="23" t="s">
+        <v>867</v>
+      </c>
+      <c r="I135" s="26" t="s">
+        <v>869</v>
+      </c>
       <c r="K135" s="29"/>
       <c r="L135" s="31"/>
       <c r="M135" s="29"/>
       <c r="N135" s="33"/>
       <c r="P135" s="29"/>
       <c r="Q135" s="32"/>
-      <c r="R135" s="27"/>
+      <c r="R135" s="34" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="136" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A136" s="27"/>
-      <c r="B136" s="39"/>
-      <c r="D136" s="31"/>
-      <c r="E136" s="33"/>
+      <c r="A136" s="19" t="s">
+        <v>870</v>
+      </c>
+      <c r="B136" s="43" t="s">
+        <v>872</v>
+      </c>
+      <c r="C136" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D136" s="23" t="s">
+        <v>871</v>
+      </c>
+      <c r="E136" s="26" t="s">
+        <v>872</v>
+      </c>
       <c r="G136" s="29"/>
-      <c r="H136" s="31"/>
-      <c r="I136" s="33"/>
+      <c r="H136" s="23" t="s">
+        <v>871</v>
+      </c>
+      <c r="I136" s="26" t="s">
+        <v>873</v>
+      </c>
       <c r="K136" s="29"/>
       <c r="L136" s="31"/>
       <c r="M136" s="29"/>
       <c r="N136" s="33"/>
       <c r="P136" s="29"/>
       <c r="Q136" s="32"/>
-      <c r="R136" s="27"/>
+      <c r="R136" s="34" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="137" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A137" s="27"/>
-      <c r="B137" s="39"/>
-      <c r="D137" s="31"/>
-      <c r="E137" s="33"/>
+      <c r="A137" s="19" t="s">
+        <v>874</v>
+      </c>
+      <c r="B137" s="43" t="s">
+        <v>876</v>
+      </c>
+      <c r="C137" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D137" s="23" t="s">
+        <v>875</v>
+      </c>
+      <c r="E137" s="26" t="s">
+        <v>876</v>
+      </c>
       <c r="G137" s="29"/>
-      <c r="H137" s="31"/>
-      <c r="I137" s="33"/>
+      <c r="H137" s="23" t="s">
+        <v>875</v>
+      </c>
+      <c r="I137" s="26" t="s">
+        <v>877</v>
+      </c>
       <c r="K137" s="29"/>
       <c r="L137" s="31"/>
       <c r="M137" s="29"/>
       <c r="N137" s="33"/>
       <c r="P137" s="29"/>
       <c r="Q137" s="32"/>
-      <c r="R137" s="27"/>
+      <c r="R137" s="34" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="138" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A138" s="27"/>
-      <c r="B138" s="39"/>
-      <c r="D138" s="31"/>
-      <c r="E138" s="33"/>
+      <c r="A138" s="19" t="s">
+        <v>878</v>
+      </c>
+      <c r="B138" s="43" t="s">
+        <v>880</v>
+      </c>
+      <c r="C138" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D138" s="23" t="s">
+        <v>879</v>
+      </c>
+      <c r="E138" s="26" t="s">
+        <v>880</v>
+      </c>
       <c r="G138" s="29"/>
-      <c r="H138" s="31"/>
-      <c r="I138" s="33"/>
+      <c r="H138" s="23" t="s">
+        <v>879</v>
+      </c>
+      <c r="I138" s="26" t="s">
+        <v>881</v>
+      </c>
       <c r="K138" s="29"/>
       <c r="L138" s="31"/>
       <c r="M138" s="29"/>
       <c r="N138" s="33"/>
       <c r="P138" s="29"/>
       <c r="Q138" s="32"/>
-      <c r="R138" s="27"/>
+      <c r="R138" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="139" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A139" s="27"/>
-      <c r="B139" s="39"/>
-      <c r="D139" s="31"/>
-      <c r="E139" s="33"/>
+      <c r="A139" s="19" t="s">
+        <v>882</v>
+      </c>
+      <c r="B139" s="43" t="s">
+        <v>884</v>
+      </c>
+      <c r="C139" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D139" s="23" t="s">
+        <v>883</v>
+      </c>
+      <c r="E139" s="26" t="s">
+        <v>884</v>
+      </c>
       <c r="G139" s="29"/>
-      <c r="H139" s="31"/>
-      <c r="I139" s="33"/>
+      <c r="H139" s="23" t="s">
+        <v>883</v>
+      </c>
+      <c r="I139" s="26" t="s">
+        <v>885</v>
+      </c>
       <c r="K139" s="29"/>
       <c r="L139" s="31"/>
       <c r="M139" s="29"/>
       <c r="N139" s="33"/>
       <c r="P139" s="29"/>
       <c r="Q139" s="32"/>
-      <c r="R139" s="27"/>
+      <c r="R139" s="34" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="140" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A140" s="27"/>
-      <c r="B140" s="39"/>
-      <c r="D140" s="31"/>
-      <c r="E140" s="33"/>
+      <c r="A140" s="19" t="s">
+        <v>886</v>
+      </c>
+      <c r="B140" s="43" t="s">
+        <v>888</v>
+      </c>
+      <c r="C140" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D140" s="23" t="s">
+        <v>887</v>
+      </c>
+      <c r="E140" s="26" t="s">
+        <v>888</v>
+      </c>
       <c r="G140" s="29"/>
-      <c r="H140" s="31"/>
-      <c r="I140" s="33"/>
+      <c r="H140" s="23" t="s">
+        <v>887</v>
+      </c>
+      <c r="I140" s="26" t="s">
+        <v>889</v>
+      </c>
       <c r="K140" s="29"/>
       <c r="L140" s="31"/>
       <c r="M140" s="29"/>
       <c r="N140" s="33"/>
       <c r="P140" s="29"/>
       <c r="Q140" s="32"/>
-      <c r="R140" s="27"/>
+      <c r="R140" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="141" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A141" s="27"/>
-      <c r="B141" s="39"/>
-      <c r="D141" s="31"/>
-      <c r="E141" s="33"/>
+      <c r="A141" s="19" t="s">
+        <v>890</v>
+      </c>
+      <c r="B141" s="43" t="s">
+        <v>892</v>
+      </c>
+      <c r="C141" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D141" s="23" t="s">
+        <v>891</v>
+      </c>
+      <c r="E141" s="26" t="s">
+        <v>892</v>
+      </c>
       <c r="G141" s="29"/>
-      <c r="H141" s="31"/>
-      <c r="I141" s="33"/>
+      <c r="H141" s="23" t="s">
+        <v>891</v>
+      </c>
+      <c r="I141" s="26" t="s">
+        <v>893</v>
+      </c>
       <c r="K141" s="29"/>
       <c r="L141" s="31"/>
       <c r="M141" s="29"/>
       <c r="N141" s="33"/>
       <c r="P141" s="29"/>
       <c r="Q141" s="32"/>
-      <c r="R141" s="27"/>
+      <c r="R141" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="142" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A142" s="27"/>
-      <c r="B142" s="39"/>
-      <c r="D142" s="31"/>
-      <c r="E142" s="33"/>
+      <c r="A142" s="27" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B142" s="69" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D142" s="70" t="s">
+        <v>1073</v>
+      </c>
+      <c r="E142" s="69" t="s">
+        <v>1115</v>
+      </c>
       <c r="G142" s="29"/>
-      <c r="H142" s="31"/>
-      <c r="I142" s="33"/>
+      <c r="H142" s="70" t="s">
+        <v>1073</v>
+      </c>
+      <c r="I142" s="69" t="s">
+        <v>1116</v>
+      </c>
       <c r="K142" s="29"/>
       <c r="L142" s="31"/>
       <c r="M142" s="29"/>
@@ -8397,13 +8751,25 @@
       <c r="R143" s="27"/>
     </row>
     <row r="144" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A144" s="27"/>
-      <c r="B144" s="39"/>
-      <c r="D144" s="31"/>
-      <c r="E144" s="33"/>
+      <c r="A144" s="27" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B144" s="79" t="s">
+        <v>1226</v>
+      </c>
+      <c r="D144" s="31" t="s">
+        <v>312</v>
+      </c>
+      <c r="E144" s="33" t="s">
+        <v>1226</v>
+      </c>
       <c r="G144" s="29"/>
-      <c r="H144" s="31"/>
-      <c r="I144" s="33"/>
+      <c r="H144" s="31" t="s">
+        <v>312</v>
+      </c>
+      <c r="I144" s="33" t="s">
+        <v>1227</v>
+      </c>
       <c r="K144" s="29"/>
       <c r="L144" s="31"/>
       <c r="M144" s="29"/>
@@ -23180,6 +23546,166 @@
       <c r="Q1067" s="32"/>
       <c r="R1067" s="27"/>
     </row>
+    <row r="1068" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1068" s="27"/>
+      <c r="B1068" s="39"/>
+      <c r="D1068" s="31"/>
+      <c r="E1068" s="33"/>
+      <c r="G1068" s="29"/>
+      <c r="H1068" s="31"/>
+      <c r="I1068" s="33"/>
+      <c r="K1068" s="29"/>
+      <c r="L1068" s="31"/>
+      <c r="M1068" s="29"/>
+      <c r="N1068" s="33"/>
+      <c r="P1068" s="29"/>
+      <c r="Q1068" s="32"/>
+      <c r="R1068" s="27"/>
+    </row>
+    <row r="1069" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1069" s="27"/>
+      <c r="B1069" s="39"/>
+      <c r="D1069" s="31"/>
+      <c r="E1069" s="33"/>
+      <c r="G1069" s="29"/>
+      <c r="H1069" s="31"/>
+      <c r="I1069" s="33"/>
+      <c r="K1069" s="29"/>
+      <c r="L1069" s="31"/>
+      <c r="M1069" s="29"/>
+      <c r="N1069" s="33"/>
+      <c r="P1069" s="29"/>
+      <c r="Q1069" s="32"/>
+      <c r="R1069" s="27"/>
+    </row>
+    <row r="1070" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1070" s="27"/>
+      <c r="B1070" s="39"/>
+      <c r="D1070" s="31"/>
+      <c r="E1070" s="33"/>
+      <c r="G1070" s="29"/>
+      <c r="H1070" s="31"/>
+      <c r="I1070" s="33"/>
+      <c r="K1070" s="29"/>
+      <c r="L1070" s="31"/>
+      <c r="M1070" s="29"/>
+      <c r="N1070" s="33"/>
+      <c r="P1070" s="29"/>
+      <c r="Q1070" s="32"/>
+      <c r="R1070" s="27"/>
+    </row>
+    <row r="1071" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1071" s="27"/>
+      <c r="B1071" s="39"/>
+      <c r="D1071" s="31"/>
+      <c r="E1071" s="33"/>
+      <c r="G1071" s="29"/>
+      <c r="H1071" s="31"/>
+      <c r="I1071" s="33"/>
+      <c r="K1071" s="29"/>
+      <c r="L1071" s="31"/>
+      <c r="M1071" s="29"/>
+      <c r="N1071" s="33"/>
+      <c r="P1071" s="29"/>
+      <c r="Q1071" s="32"/>
+      <c r="R1071" s="27"/>
+    </row>
+    <row r="1072" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1072" s="27"/>
+      <c r="B1072" s="39"/>
+      <c r="D1072" s="31"/>
+      <c r="E1072" s="33"/>
+      <c r="G1072" s="29"/>
+      <c r="H1072" s="31"/>
+      <c r="I1072" s="33"/>
+      <c r="K1072" s="29"/>
+      <c r="L1072" s="31"/>
+      <c r="M1072" s="29"/>
+      <c r="N1072" s="33"/>
+      <c r="P1072" s="29"/>
+      <c r="Q1072" s="32"/>
+      <c r="R1072" s="27"/>
+    </row>
+    <row r="1073" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1073" s="27"/>
+      <c r="B1073" s="39"/>
+      <c r="D1073" s="31"/>
+      <c r="E1073" s="33"/>
+      <c r="G1073" s="29"/>
+      <c r="H1073" s="31"/>
+      <c r="I1073" s="33"/>
+      <c r="K1073" s="29"/>
+      <c r="L1073" s="31"/>
+      <c r="M1073" s="29"/>
+      <c r="N1073" s="33"/>
+      <c r="P1073" s="29"/>
+      <c r="Q1073" s="32"/>
+      <c r="R1073" s="27"/>
+    </row>
+    <row r="1074" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1074" s="27"/>
+      <c r="B1074" s="39"/>
+      <c r="D1074" s="31"/>
+      <c r="E1074" s="33"/>
+      <c r="G1074" s="29"/>
+      <c r="H1074" s="31"/>
+      <c r="I1074" s="33"/>
+      <c r="K1074" s="29"/>
+      <c r="L1074" s="31"/>
+      <c r="M1074" s="29"/>
+      <c r="N1074" s="33"/>
+      <c r="P1074" s="29"/>
+      <c r="Q1074" s="32"/>
+      <c r="R1074" s="27"/>
+    </row>
+    <row r="1075" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1075" s="27"/>
+      <c r="B1075" s="39"/>
+      <c r="D1075" s="31"/>
+      <c r="E1075" s="33"/>
+      <c r="G1075" s="29"/>
+      <c r="H1075" s="31"/>
+      <c r="I1075" s="33"/>
+      <c r="K1075" s="29"/>
+      <c r="L1075" s="31"/>
+      <c r="M1075" s="29"/>
+      <c r="N1075" s="33"/>
+      <c r="P1075" s="29"/>
+      <c r="Q1075" s="32"/>
+      <c r="R1075" s="27"/>
+    </row>
+    <row r="1076" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1076" s="27"/>
+      <c r="B1076" s="39"/>
+      <c r="D1076" s="31"/>
+      <c r="E1076" s="33"/>
+      <c r="G1076" s="29"/>
+      <c r="H1076" s="31"/>
+      <c r="I1076" s="33"/>
+      <c r="K1076" s="29"/>
+      <c r="L1076" s="31"/>
+      <c r="M1076" s="29"/>
+      <c r="N1076" s="33"/>
+      <c r="P1076" s="29"/>
+      <c r="Q1076" s="32"/>
+      <c r="R1076" s="27"/>
+    </row>
+    <row r="1077" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1077" s="27"/>
+      <c r="B1077" s="39"/>
+      <c r="D1077" s="31"/>
+      <c r="E1077" s="33"/>
+      <c r="G1077" s="29"/>
+      <c r="H1077" s="31"/>
+      <c r="I1077" s="33"/>
+      <c r="K1077" s="29"/>
+      <c r="L1077" s="31"/>
+      <c r="M1077" s="29"/>
+      <c r="N1077" s="33"/>
+      <c r="P1077" s="29"/>
+      <c r="Q1077" s="32"/>
+      <c r="R1077" s="27"/>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -23194,27 +23720,27 @@
   </sheetPr>
   <dimension ref="A1:AB1016"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+    <sheetView zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="19.46484375" style="62" customWidth="1"/>
+    <col min="2" max="2" width="19.3984375" style="62" customWidth="1"/>
     <col min="3" max="3" width="40.265625" customWidth="1"/>
     <col min="4" max="4" width="53.1328125" customWidth="1"/>
-    <col min="5" max="5" width="18.46484375" customWidth="1"/>
+    <col min="5" max="5" width="18.3984375" customWidth="1"/>
     <col min="6" max="6" width="6.1328125" customWidth="1"/>
-    <col min="7" max="7" width="6.46484375" customWidth="1"/>
-    <col min="8" max="8" width="40.53125" customWidth="1"/>
-    <col min="10" max="11" width="6.46484375" customWidth="1"/>
-    <col min="12" max="12" width="16.46484375" customWidth="1"/>
-    <col min="13" max="13" width="34.53125" customWidth="1"/>
-    <col min="14" max="14" width="18.796875" customWidth="1"/>
+    <col min="7" max="7" width="6.3984375" customWidth="1"/>
+    <col min="8" max="8" width="40.59765625" customWidth="1"/>
+    <col min="10" max="11" width="6.3984375" customWidth="1"/>
+    <col min="12" max="12" width="16.3984375" customWidth="1"/>
+    <col min="13" max="13" width="34.59765625" customWidth="1"/>
+    <col min="14" max="14" width="18.86328125" customWidth="1"/>
     <col min="15" max="15" width="6" customWidth="1"/>
     <col min="16" max="16" width="7.1328125" customWidth="1"/>
-    <col min="17" max="17" width="94.46484375" customWidth="1"/>
+    <col min="17" max="17" width="94.3984375" customWidth="1"/>
     <col min="18" max="18" width="122.265625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -39506,22 +40032,22 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A23" sqref="A23:XFD23"/>
+      <selection pane="topRight" activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="19.796875" customWidth="1"/>
+    <col min="2" max="2" width="19.86328125" customWidth="1"/>
     <col min="3" max="3" width="36.73046875" customWidth="1"/>
-    <col min="4" max="4" width="40.46484375" customWidth="1"/>
+    <col min="4" max="4" width="40.3984375" customWidth="1"/>
     <col min="5" max="5" width="19.73046875" customWidth="1"/>
     <col min="6" max="6" width="6.73046875" customWidth="1"/>
-    <col min="7" max="7" width="6.53125" customWidth="1"/>
+    <col min="7" max="7" width="6.59765625" customWidth="1"/>
     <col min="8" max="8" width="37.73046875" customWidth="1"/>
-    <col min="10" max="11" width="6.46484375" customWidth="1"/>
+    <col min="10" max="11" width="6.3984375" customWidth="1"/>
     <col min="12" max="14" width="18.1328125" customWidth="1"/>
     <col min="15" max="16" width="6.265625" customWidth="1"/>
-    <col min="17" max="17" width="59.46484375" customWidth="1"/>
+    <col min="17" max="17" width="59.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -40771,18 +41297,18 @@
       <c r="A39" s="35" t="s">
         <v>1129</v>
       </c>
-      <c r="B39" s="72" t="s">
+      <c r="B39" s="71" t="s">
         <v>1138</v>
       </c>
-      <c r="D39" s="72" t="s">
+      <c r="D39" s="71" t="s">
         <v>1132</v>
       </c>
-      <c r="E39" s="72" t="s">
+      <c r="E39" s="71" t="s">
         <v>1138</v>
       </c>
       <c r="F39" s="25"/>
       <c r="G39" s="27"/>
-      <c r="H39" s="72" t="s">
+      <c r="H39" s="71" t="s">
         <v>1132</v>
       </c>
       <c r="I39" s="27" t="s">
@@ -40801,19 +41327,19 @@
       <c r="A40" s="45" t="s">
         <v>1130</v>
       </c>
-      <c r="B40" s="72" t="s">
+      <c r="B40" s="71" t="s">
         <v>1139</v>
       </c>
       <c r="C40" s="62"/>
-      <c r="D40" s="74" t="s">
+      <c r="D40" s="73" t="s">
         <v>1133</v>
       </c>
-      <c r="E40" s="72" t="s">
+      <c r="E40" s="71" t="s">
         <v>1139</v>
       </c>
       <c r="F40" s="25"/>
       <c r="G40" s="27"/>
-      <c r="H40" s="72" t="s">
+      <c r="H40" s="71" t="s">
         <v>1133</v>
       </c>
       <c r="I40" s="27" t="s">
@@ -40832,19 +41358,19 @@
       <c r="A41" s="35" t="s">
         <v>1131</v>
       </c>
-      <c r="B41" s="72" t="s">
+      <c r="B41" s="71" t="s">
         <v>1135</v>
       </c>
       <c r="C41" s="62"/>
-      <c r="D41" s="73" t="s">
+      <c r="D41" s="72" t="s">
         <v>1134</v>
       </c>
-      <c r="E41" s="72" t="s">
+      <c r="E41" s="71" t="s">
         <v>1135</v>
       </c>
       <c r="F41" s="25"/>
       <c r="G41" s="27"/>
-      <c r="H41" s="73" t="s">
+      <c r="H41" s="72" t="s">
         <v>1134</v>
       </c>
       <c r="I41" s="27" t="s">
@@ -59112,27 +59638,27 @@
   </sheetPr>
   <dimension ref="A1:AB1030"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.46484375" style="57"/>
+    <col min="1" max="1" width="14.3984375" style="57"/>
     <col min="2" max="2" width="28.1328125" customWidth="1"/>
-    <col min="3" max="3" width="40.53125" customWidth="1"/>
+    <col min="3" max="3" width="40.59765625" customWidth="1"/>
     <col min="4" max="4" width="34.73046875" customWidth="1"/>
     <col min="5" max="5" width="20.265625" customWidth="1"/>
     <col min="6" max="6" width="6.1328125" customWidth="1"/>
     <col min="7" max="7" width="6.265625" customWidth="1"/>
     <col min="8" max="8" width="41.1328125" customWidth="1"/>
-    <col min="10" max="10" width="5.46484375" customWidth="1"/>
-    <col min="11" max="11" width="6.46484375" customWidth="1"/>
+    <col min="10" max="10" width="5.3984375" customWidth="1"/>
+    <col min="11" max="11" width="6.3984375" customWidth="1"/>
     <col min="12" max="12" width="16.265625" customWidth="1"/>
     <col min="13" max="13" width="27.265625" customWidth="1"/>
     <col min="14" max="14" width="16.73046875" customWidth="1"/>
     <col min="15" max="15" width="6" customWidth="1"/>
-    <col min="16" max="16" width="6.46484375" customWidth="1"/>
+    <col min="16" max="16" width="6.3984375" customWidth="1"/>
     <col min="17" max="17" width="62.265625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -59813,7 +60339,7 @@
       <c r="A23" s="35" t="s">
         <v>981</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="76" t="s">
         <v>984</v>
       </c>
       <c r="C23" s="19" t="s">
@@ -60390,11 +60916,28 @@
       <c r="Q44" s="32"/>
     </row>
     <row r="45" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B45" s="27"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="25"/>
+      <c r="A45" s="57" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B45" s="27" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C45" s="32" t="s">
+        <v>1210</v>
+      </c>
+      <c r="D45" s="41" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>1208</v>
+      </c>
       <c r="F45" s="30"/>
-      <c r="H45" s="30"/>
+      <c r="H45" s="30" t="s">
+        <v>1207</v>
+      </c>
+      <c r="I45" s="21" t="s">
+        <v>1209</v>
+      </c>
       <c r="J45" s="30"/>
       <c r="L45" s="30"/>
       <c r="M45" s="25"/>
@@ -60402,8 +60945,13 @@
       <c r="Q45" s="32"/>
     </row>
     <row r="46" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A46" s="57" t="s">
+        <v>1219</v>
+      </c>
       <c r="B46" s="27"/>
-      <c r="C46" s="32"/>
+      <c r="C46" s="32" t="s">
+        <v>1220</v>
+      </c>
       <c r="D46" s="25"/>
       <c r="F46" s="30"/>
       <c r="H46" s="30"/>

</xml_diff>

<commit_message>
added terms for lung connectivity
</commit_message>
<xml_diff>
--- a/anatomical-map/flatmap_annotation.xlsx
+++ b/anatomical-map/flatmap_annotation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nebr002\work\sparc\flatmaps-wip\rat\powerpoint\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nebr002\work\sparc\flatmaps\anatomical-map\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2016" uniqueCount="1228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2094" uniqueCount="1276">
   <si>
     <t>Power point identifier</t>
   </si>
@@ -3708,6 +3708,150 @@
   </si>
   <si>
     <t>ILX:0101359</t>
+  </si>
+  <si>
+    <t>respiratory_15</t>
+  </si>
+  <si>
+    <t>respiratory airway</t>
+  </si>
+  <si>
+    <t>UBERON:0001005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILX:0728555 </t>
+  </si>
+  <si>
+    <t>respiratory_16</t>
+  </si>
+  <si>
+    <t>respiratory_17</t>
+  </si>
+  <si>
+    <t>respiratory_18</t>
+  </si>
+  <si>
+    <t>respiratory_19</t>
+  </si>
+  <si>
+    <t>smooth muscle tissue of terminal bronchiole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBERON:0004516 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILX:0727052  </t>
+  </si>
+  <si>
+    <t>smooth muscle tissue of bronchiole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBERON:0004515 </t>
+  </si>
+  <si>
+    <t>ILX:0730859</t>
+  </si>
+  <si>
+    <t>bronchus smooth muscle</t>
+  </si>
+  <si>
+    <t>UBERON:0004242</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILX:0728214  </t>
+  </si>
+  <si>
+    <t>smooth muscle of trachea</t>
+  </si>
+  <si>
+    <t>UBERON:0003387</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILX:0724686 </t>
+  </si>
+  <si>
+    <t>receptor_1</t>
+  </si>
+  <si>
+    <t>receptor_2</t>
+  </si>
+  <si>
+    <t>Acetylcholine (muscarinic) receptor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILX:0100241 </t>
+  </si>
+  <si>
+    <t>Beta2 receptor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILX:0101253 </t>
+  </si>
+  <si>
+    <t>Nicotinic Acetylcholine Receptor</t>
+  </si>
+  <si>
+    <t>receptor_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILX:0107579  </t>
+  </si>
+  <si>
+    <t>endocrine_4</t>
+  </si>
+  <si>
+    <t>endocrine_5</t>
+  </si>
+  <si>
+    <t>endocrine_6</t>
+  </si>
+  <si>
+    <t>chromaffin cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILX:0102147 </t>
+  </si>
+  <si>
+    <t>adrenal gland cortex zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBERON:0009753 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILX:0731630 </t>
+  </si>
+  <si>
+    <t>adrenal medulla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBERON:0001236 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILX:0730114  </t>
+  </si>
+  <si>
+    <t>lung_1</t>
+  </si>
+  <si>
+    <t>parasympathetic ganglion</t>
+  </si>
+  <si>
+    <t>UBERON:0001808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILX:0734328 </t>
+  </si>
+  <si>
+    <t>lung_2</t>
+  </si>
+  <si>
+    <t>splanchnic nerve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBERON:0003715 </t>
+  </si>
+  <si>
+    <t>ILX:0730942</t>
   </si>
 </sst>
 </file>
@@ -4042,7 +4186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -4169,6 +4313,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4387,10 +4538,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB1077"/>
+  <dimension ref="A1:AB1085"/>
   <sheetViews>
-    <sheetView topLeftCell="A115" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
-      <selection activeCell="A144" sqref="A144"/>
+    <sheetView topLeftCell="A118" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
+      <selection activeCell="A140" sqref="A140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -6657,14 +6808,26 @@
       <c r="R73" s="40"/>
     </row>
     <row r="74" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A74" s="19"/>
-      <c r="B74" s="39"/>
+      <c r="A74" s="35" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B74" s="35" t="s">
+        <v>1230</v>
+      </c>
       <c r="C74" s="21"/>
-      <c r="D74" s="23"/>
-      <c r="E74" s="26"/>
+      <c r="D74" s="67" t="s">
+        <v>1229</v>
+      </c>
+      <c r="E74" s="43" t="s">
+        <v>1230</v>
+      </c>
       <c r="G74" s="29"/>
-      <c r="H74" s="23"/>
-      <c r="I74" s="26"/>
+      <c r="H74" s="67" t="s">
+        <v>1229</v>
+      </c>
+      <c r="I74" s="68" t="s">
+        <v>1231</v>
+      </c>
       <c r="K74" s="29"/>
       <c r="L74" s="31"/>
       <c r="M74" s="29"/>
@@ -6674,27 +6837,25 @@
       <c r="R74" s="40"/>
     </row>
     <row r="75" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A75" s="19" t="s">
-        <v>760</v>
-      </c>
-      <c r="B75" s="43" t="s">
-        <v>762</v>
-      </c>
-      <c r="C75" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D75" s="23" t="s">
-        <v>761</v>
-      </c>
-      <c r="E75" s="26" t="s">
-        <v>762</v>
+      <c r="A75" s="35" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B75" s="65" t="s">
+        <v>1246</v>
+      </c>
+      <c r="C75" s="21"/>
+      <c r="D75" s="67" t="s">
+        <v>1245</v>
+      </c>
+      <c r="E75" s="68" t="s">
+        <v>1246</v>
       </c>
       <c r="G75" s="29"/>
-      <c r="H75" s="42" t="s">
-        <v>761</v>
-      </c>
-      <c r="I75" s="26" t="s">
-        <v>763</v>
+      <c r="H75" s="67" t="s">
+        <v>1245</v>
+      </c>
+      <c r="I75" s="68" t="s">
+        <v>1247</v>
       </c>
       <c r="K75" s="29"/>
       <c r="L75" s="31"/>
@@ -6702,32 +6863,28 @@
       <c r="N75" s="33"/>
       <c r="P75" s="29"/>
       <c r="Q75" s="32"/>
-      <c r="R75" s="34" t="s">
-        <v>764</v>
-      </c>
+      <c r="R75" s="40"/>
     </row>
     <row r="76" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A76" s="19" t="s">
-        <v>765</v>
-      </c>
-      <c r="B76" s="43" t="s">
-        <v>767</v>
-      </c>
-      <c r="C76" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D76" s="23" t="s">
-        <v>766</v>
-      </c>
-      <c r="E76" s="26" t="s">
-        <v>767</v>
+      <c r="A76" s="35" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B76" s="65" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C76" s="21"/>
+      <c r="D76" s="67" t="s">
+        <v>1242</v>
+      </c>
+      <c r="E76" s="68" t="s">
+        <v>1243</v>
       </c>
       <c r="G76" s="29"/>
-      <c r="H76" s="23" t="s">
-        <v>766</v>
-      </c>
-      <c r="I76" s="26" t="s">
-        <v>768</v>
+      <c r="H76" s="67" t="s">
+        <v>1242</v>
+      </c>
+      <c r="I76" s="68" t="s">
+        <v>1244</v>
       </c>
       <c r="K76" s="29"/>
       <c r="L76" s="31"/>
@@ -6735,32 +6892,28 @@
       <c r="N76" s="33"/>
       <c r="P76" s="29"/>
       <c r="Q76" s="32"/>
-      <c r="R76" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R76" s="40"/>
     </row>
     <row r="77" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A77" s="19" t="s">
-        <v>769</v>
-      </c>
-      <c r="B77" s="43" t="s">
-        <v>771</v>
-      </c>
-      <c r="C77" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D77" s="42" t="s">
-        <v>770</v>
-      </c>
-      <c r="E77" s="26" t="s">
-        <v>771</v>
+      <c r="A77" s="35" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B77" s="65" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C77" s="21"/>
+      <c r="D77" s="67" t="s">
+        <v>1239</v>
+      </c>
+      <c r="E77" s="68" t="s">
+        <v>1240</v>
       </c>
       <c r="G77" s="29"/>
-      <c r="H77" s="42" t="s">
-        <v>770</v>
-      </c>
-      <c r="I77" s="26" t="s">
-        <v>772</v>
+      <c r="H77" s="67" t="s">
+        <v>1239</v>
+      </c>
+      <c r="I77" s="68" t="s">
+        <v>1241</v>
       </c>
       <c r="K77" s="29"/>
       <c r="L77" s="31"/>
@@ -6768,32 +6921,28 @@
       <c r="N77" s="33"/>
       <c r="P77" s="29"/>
       <c r="Q77" s="32"/>
-      <c r="R77" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R77" s="40"/>
     </row>
     <row r="78" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A78" s="19" t="s">
-        <v>773</v>
-      </c>
-      <c r="B78" s="43" t="s">
-        <v>775</v>
-      </c>
-      <c r="C78" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D78" s="42" t="s">
-        <v>774</v>
-      </c>
-      <c r="E78" s="26" t="s">
-        <v>775</v>
+      <c r="A78" s="65" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B78" s="65" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C78" s="21"/>
+      <c r="D78" s="67" t="s">
+        <v>1236</v>
+      </c>
+      <c r="E78" s="68" t="s">
+        <v>1237</v>
       </c>
       <c r="G78" s="29"/>
-      <c r="H78" s="42" t="s">
-        <v>774</v>
-      </c>
-      <c r="I78" s="26" t="s">
-        <v>776</v>
+      <c r="H78" s="67" t="s">
+        <v>1236</v>
+      </c>
+      <c r="I78" s="68" t="s">
+        <v>1238</v>
       </c>
       <c r="K78" s="29"/>
       <c r="L78" s="31"/>
@@ -6801,65 +6950,47 @@
       <c r="N78" s="33"/>
       <c r="P78" s="29"/>
       <c r="Q78" s="32"/>
-      <c r="R78" s="34" t="s">
-        <v>95</v>
-      </c>
+      <c r="R78" s="40"/>
     </row>
     <row r="79" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A79" s="19" t="s">
-        <v>777</v>
-      </c>
-      <c r="B79" s="43" t="s">
-        <v>779</v>
-      </c>
-      <c r="C79" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D79" s="23" t="s">
-        <v>778</v>
-      </c>
-      <c r="E79" s="26" t="s">
-        <v>779</v>
-      </c>
+      <c r="A79" s="19"/>
+      <c r="B79" s="39"/>
+      <c r="C79" s="21"/>
+      <c r="D79" s="23"/>
+      <c r="E79" s="26"/>
       <c r="G79" s="29"/>
-      <c r="H79" s="23" t="s">
-        <v>778</v>
-      </c>
-      <c r="I79" s="26" t="s">
-        <v>780</v>
-      </c>
+      <c r="H79" s="23"/>
+      <c r="I79" s="26"/>
       <c r="K79" s="29"/>
       <c r="L79" s="31"/>
       <c r="M79" s="29"/>
       <c r="N79" s="33"/>
       <c r="P79" s="29"/>
       <c r="Q79" s="32"/>
-      <c r="R79" s="34" t="s">
-        <v>33</v>
-      </c>
+      <c r="R79" s="40"/>
     </row>
     <row r="80" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A80" s="19" t="s">
-        <v>781</v>
+        <v>760</v>
       </c>
       <c r="B80" s="43" t="s">
-        <v>783</v>
+        <v>762</v>
       </c>
       <c r="C80" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D80" s="23" t="s">
-        <v>782</v>
+        <v>761</v>
       </c>
       <c r="E80" s="26" t="s">
-        <v>783</v>
+        <v>762</v>
       </c>
       <c r="G80" s="29"/>
-      <c r="H80" s="23" t="s">
-        <v>782</v>
+      <c r="H80" s="42" t="s">
+        <v>761</v>
       </c>
       <c r="I80" s="26" t="s">
-        <v>784</v>
+        <v>763</v>
       </c>
       <c r="K80" s="29"/>
       <c r="L80" s="31"/>
@@ -6867,32 +6998,32 @@
       <c r="N80" s="33"/>
       <c r="P80" s="29"/>
       <c r="Q80" s="32"/>
-      <c r="R80" s="34" t="b">
-        <v>1</v>
+      <c r="R80" s="34" t="s">
+        <v>764</v>
       </c>
     </row>
     <row r="81" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A81" s="19" t="s">
-        <v>785</v>
+        <v>765</v>
       </c>
       <c r="B81" s="43" t="s">
-        <v>787</v>
+        <v>767</v>
       </c>
       <c r="C81" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D81" s="23" t="s">
-        <v>786</v>
+        <v>766</v>
       </c>
       <c r="E81" s="26" t="s">
-        <v>787</v>
+        <v>767</v>
       </c>
       <c r="G81" s="29"/>
       <c r="H81" s="23" t="s">
-        <v>786</v>
+        <v>766</v>
       </c>
       <c r="I81" s="26" t="s">
-        <v>788</v>
+        <v>768</v>
       </c>
       <c r="K81" s="29"/>
       <c r="L81" s="31"/>
@@ -6906,26 +7037,26 @@
     </row>
     <row r="82" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A82" s="19" t="s">
-        <v>789</v>
+        <v>769</v>
       </c>
       <c r="B82" s="43" t="s">
-        <v>791</v>
+        <v>771</v>
       </c>
       <c r="C82" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D82" s="23" t="s">
-        <v>790</v>
+      <c r="D82" s="42" t="s">
+        <v>770</v>
       </c>
       <c r="E82" s="26" t="s">
-        <v>791</v>
+        <v>771</v>
       </c>
       <c r="G82" s="29"/>
-      <c r="H82" s="23" t="s">
-        <v>790</v>
+      <c r="H82" s="42" t="s">
+        <v>770</v>
       </c>
       <c r="I82" s="26" t="s">
-        <v>792</v>
+        <v>772</v>
       </c>
       <c r="K82" s="29"/>
       <c r="L82" s="31"/>
@@ -6933,32 +7064,32 @@
       <c r="N82" s="33"/>
       <c r="P82" s="29"/>
       <c r="Q82" s="32"/>
-      <c r="R82" s="34" t="s">
-        <v>33</v>
+      <c r="R82" s="34" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A83" s="19" t="s">
-        <v>793</v>
+        <v>773</v>
       </c>
       <c r="B83" s="43" t="s">
-        <v>795</v>
+        <v>775</v>
       </c>
       <c r="C83" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D83" s="23" t="s">
-        <v>794</v>
+      <c r="D83" s="42" t="s">
+        <v>774</v>
       </c>
       <c r="E83" s="26" t="s">
-        <v>795</v>
+        <v>775</v>
       </c>
       <c r="G83" s="29"/>
-      <c r="H83" s="23" t="s">
-        <v>794</v>
+      <c r="H83" s="42" t="s">
+        <v>774</v>
       </c>
       <c r="I83" s="26" t="s">
-        <v>796</v>
+        <v>776</v>
       </c>
       <c r="K83" s="29"/>
       <c r="L83" s="31"/>
@@ -6966,32 +7097,32 @@
       <c r="N83" s="33"/>
       <c r="P83" s="29"/>
       <c r="Q83" s="32"/>
-      <c r="R83" s="34" t="b">
-        <v>1</v>
+      <c r="R83" s="34" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="84" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A84" s="19" t="s">
-        <v>797</v>
+        <v>777</v>
       </c>
       <c r="B84" s="43" t="s">
-        <v>799</v>
+        <v>779</v>
       </c>
       <c r="C84" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D84" s="23" t="s">
-        <v>798</v>
+        <v>778</v>
       </c>
       <c r="E84" s="26" t="s">
-        <v>799</v>
+        <v>779</v>
       </c>
       <c r="G84" s="29"/>
       <c r="H84" s="23" t="s">
-        <v>798</v>
+        <v>778</v>
       </c>
       <c r="I84" s="26" t="s">
-        <v>800</v>
+        <v>780</v>
       </c>
       <c r="K84" s="29"/>
       <c r="L84" s="31"/>
@@ -6999,32 +7130,32 @@
       <c r="N84" s="33"/>
       <c r="P84" s="29"/>
       <c r="Q84" s="32"/>
-      <c r="R84" s="34" t="b">
-        <v>1</v>
+      <c r="R84" s="34" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="85" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A85" s="19" t="s">
-        <v>801</v>
+        <v>781</v>
       </c>
       <c r="B85" s="43" t="s">
-        <v>804</v>
-      </c>
-      <c r="C85" s="50" t="s">
-        <v>802</v>
+        <v>783</v>
+      </c>
+      <c r="C85" s="21" t="s">
+        <v>20</v>
       </c>
       <c r="D85" s="23" t="s">
-        <v>803</v>
+        <v>782</v>
       </c>
       <c r="E85" s="26" t="s">
-        <v>804</v>
+        <v>783</v>
       </c>
       <c r="G85" s="29"/>
       <c r="H85" s="23" t="s">
-        <v>803</v>
+        <v>782</v>
       </c>
       <c r="I85" s="26" t="s">
-        <v>805</v>
+        <v>784</v>
       </c>
       <c r="K85" s="29"/>
       <c r="L85" s="31"/>
@@ -7038,26 +7169,26 @@
     </row>
     <row r="86" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A86" s="19" t="s">
-        <v>806</v>
+        <v>785</v>
       </c>
       <c r="B86" s="43" t="s">
-        <v>809</v>
-      </c>
-      <c r="C86" s="50" t="s">
-        <v>807</v>
+        <v>787</v>
+      </c>
+      <c r="C86" s="21" t="s">
+        <v>20</v>
       </c>
       <c r="D86" s="23" t="s">
-        <v>808</v>
+        <v>786</v>
       </c>
       <c r="E86" s="26" t="s">
-        <v>809</v>
+        <v>787</v>
       </c>
       <c r="G86" s="29"/>
       <c r="H86" s="23" t="s">
-        <v>808</v>
+        <v>786</v>
       </c>
       <c r="I86" s="26" t="s">
-        <v>810</v>
+        <v>788</v>
       </c>
       <c r="K86" s="29"/>
       <c r="L86" s="31"/>
@@ -7071,26 +7202,26 @@
     </row>
     <row r="87" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A87" s="19" t="s">
-        <v>811</v>
+        <v>789</v>
       </c>
       <c r="B87" s="43" t="s">
-        <v>813</v>
-      </c>
-      <c r="C87" s="19" t="s">
+        <v>791</v>
+      </c>
+      <c r="C87" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D87" s="21" t="s">
-        <v>812</v>
+      <c r="D87" s="23" t="s">
+        <v>790</v>
       </c>
       <c r="E87" s="26" t="s">
-        <v>813</v>
+        <v>791</v>
       </c>
       <c r="G87" s="29"/>
       <c r="H87" s="23" t="s">
-        <v>812</v>
+        <v>790</v>
       </c>
       <c r="I87" s="26" t="s">
-        <v>814</v>
+        <v>792</v>
       </c>
       <c r="K87" s="29"/>
       <c r="L87" s="31"/>
@@ -7098,32 +7229,32 @@
       <c r="N87" s="33"/>
       <c r="P87" s="29"/>
       <c r="Q87" s="32"/>
-      <c r="R87" s="34" t="b">
-        <v>1</v>
+      <c r="R87" s="34" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="88" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A88" s="19" t="s">
-        <v>815</v>
+        <v>793</v>
       </c>
       <c r="B88" s="43" t="s">
-        <v>817</v>
-      </c>
-      <c r="C88" s="19" t="s">
+        <v>795</v>
+      </c>
+      <c r="C88" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D88" s="21" t="s">
-        <v>816</v>
+      <c r="D88" s="23" t="s">
+        <v>794</v>
       </c>
       <c r="E88" s="26" t="s">
-        <v>817</v>
+        <v>795</v>
       </c>
       <c r="G88" s="29"/>
       <c r="H88" s="23" t="s">
-        <v>816</v>
+        <v>794</v>
       </c>
       <c r="I88" s="26" t="s">
-        <v>818</v>
+        <v>796</v>
       </c>
       <c r="K88" s="29"/>
       <c r="L88" s="31"/>
@@ -7137,26 +7268,26 @@
     </row>
     <row r="89" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A89" s="19" t="s">
-        <v>819</v>
+        <v>797</v>
       </c>
       <c r="B89" s="43" t="s">
-        <v>821</v>
-      </c>
-      <c r="C89" s="19" t="s">
+        <v>799</v>
+      </c>
+      <c r="C89" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D89" s="21" t="s">
-        <v>820</v>
+      <c r="D89" s="23" t="s">
+        <v>798</v>
       </c>
       <c r="E89" s="26" t="s">
-        <v>821</v>
+        <v>799</v>
       </c>
       <c r="G89" s="29"/>
       <c r="H89" s="23" t="s">
-        <v>820</v>
+        <v>798</v>
       </c>
       <c r="I89" s="26" t="s">
-        <v>822</v>
+        <v>800</v>
       </c>
       <c r="K89" s="29"/>
       <c r="L89" s="31"/>
@@ -7170,26 +7301,26 @@
     </row>
     <row r="90" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A90" s="19" t="s">
-        <v>823</v>
+        <v>801</v>
       </c>
       <c r="B90" s="43" t="s">
-        <v>825</v>
-      </c>
-      <c r="C90" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D90" s="21" t="s">
-        <v>824</v>
+        <v>804</v>
+      </c>
+      <c r="C90" s="50" t="s">
+        <v>802</v>
+      </c>
+      <c r="D90" s="23" t="s">
+        <v>803</v>
       </c>
       <c r="E90" s="26" t="s">
-        <v>825</v>
+        <v>804</v>
       </c>
       <c r="G90" s="29"/>
       <c r="H90" s="23" t="s">
-        <v>824</v>
+        <v>803</v>
       </c>
       <c r="I90" s="26" t="s">
-        <v>826</v>
+        <v>805</v>
       </c>
       <c r="K90" s="29"/>
       <c r="L90" s="31"/>
@@ -7197,32 +7328,32 @@
       <c r="N90" s="33"/>
       <c r="P90" s="29"/>
       <c r="Q90" s="32"/>
-      <c r="R90" s="34" t="s">
-        <v>827</v>
+      <c r="R90" s="34" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A91" s="19" t="s">
-        <v>828</v>
+        <v>806</v>
       </c>
       <c r="B91" s="43" t="s">
-        <v>830</v>
-      </c>
-      <c r="C91" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D91" s="21" t="s">
-        <v>829</v>
+        <v>809</v>
+      </c>
+      <c r="C91" s="50" t="s">
+        <v>807</v>
+      </c>
+      <c r="D91" s="23" t="s">
+        <v>808</v>
       </c>
       <c r="E91" s="26" t="s">
-        <v>830</v>
+        <v>809</v>
       </c>
       <c r="G91" s="29"/>
       <c r="H91" s="23" t="s">
-        <v>829</v>
+        <v>808</v>
       </c>
       <c r="I91" s="26" t="s">
-        <v>831</v>
+        <v>810</v>
       </c>
       <c r="K91" s="29"/>
       <c r="L91" s="31"/>
@@ -7230,32 +7361,32 @@
       <c r="N91" s="33"/>
       <c r="P91" s="29"/>
       <c r="Q91" s="32"/>
-      <c r="R91" s="34" t="s">
-        <v>832</v>
+      <c r="R91" s="34" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A92" s="65" t="s">
-        <v>1060</v>
+      <c r="A92" s="19" t="s">
+        <v>811</v>
       </c>
       <c r="B92" s="43" t="s">
-        <v>1078</v>
-      </c>
-      <c r="C92" s="76" t="s">
+        <v>813</v>
+      </c>
+      <c r="C92" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D92" s="21" t="s">
-        <v>1077</v>
-      </c>
-      <c r="E92" s="43" t="s">
-        <v>1078</v>
-      </c>
-      <c r="G92" s="77"/>
-      <c r="H92" s="21" t="s">
-        <v>1077</v>
-      </c>
-      <c r="I92" s="43" t="s">
-        <v>1079</v>
+        <v>812</v>
+      </c>
+      <c r="E92" s="26" t="s">
+        <v>813</v>
+      </c>
+      <c r="G92" s="29"/>
+      <c r="H92" s="23" t="s">
+        <v>812</v>
+      </c>
+      <c r="I92" s="26" t="s">
+        <v>814</v>
       </c>
       <c r="K92" s="29"/>
       <c r="L92" s="31"/>
@@ -7263,30 +7394,32 @@
       <c r="N92" s="33"/>
       <c r="P92" s="29"/>
       <c r="Q92" s="32"/>
-      <c r="R92" s="40"/>
+      <c r="R92" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="93" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A93" s="35" t="s">
-        <v>1061</v>
+      <c r="A93" s="19" t="s">
+        <v>815</v>
       </c>
       <c r="B93" s="43" t="s">
-        <v>1064</v>
-      </c>
-      <c r="C93" s="76" t="s">
+        <v>817</v>
+      </c>
+      <c r="C93" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D93" s="21" t="s">
-        <v>1063</v>
-      </c>
-      <c r="E93" s="43" t="s">
-        <v>1064</v>
-      </c>
-      <c r="G93" s="77"/>
-      <c r="H93" s="21" t="s">
-        <v>1063</v>
-      </c>
-      <c r="I93" s="43" t="s">
-        <v>1080</v>
+        <v>816</v>
+      </c>
+      <c r="E93" s="26" t="s">
+        <v>817</v>
+      </c>
+      <c r="G93" s="29"/>
+      <c r="H93" s="23" t="s">
+        <v>816</v>
+      </c>
+      <c r="I93" s="26" t="s">
+        <v>818</v>
       </c>
       <c r="K93" s="29"/>
       <c r="L93" s="31"/>
@@ -7294,30 +7427,32 @@
       <c r="N93" s="33"/>
       <c r="P93" s="29"/>
       <c r="Q93" s="32"/>
-      <c r="R93" s="40"/>
+      <c r="R93" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="94" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A94" s="35" t="s">
-        <v>1062</v>
+      <c r="A94" s="19" t="s">
+        <v>819</v>
       </c>
       <c r="B94" s="43" t="s">
-        <v>1067</v>
-      </c>
-      <c r="C94" s="76" t="s">
+        <v>821</v>
+      </c>
+      <c r="C94" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D94" s="21" t="s">
-        <v>1065</v>
-      </c>
-      <c r="E94" s="43" t="s">
-        <v>1067</v>
-      </c>
-      <c r="G94" s="77"/>
-      <c r="H94" s="21" t="s">
-        <v>1065</v>
-      </c>
-      <c r="I94" s="43" t="s">
-        <v>1066</v>
+        <v>820</v>
+      </c>
+      <c r="E94" s="26" t="s">
+        <v>821</v>
+      </c>
+      <c r="G94" s="29"/>
+      <c r="H94" s="23" t="s">
+        <v>820</v>
+      </c>
+      <c r="I94" s="26" t="s">
+        <v>822</v>
       </c>
       <c r="K94" s="29"/>
       <c r="L94" s="31"/>
@@ -7325,30 +7460,32 @@
       <c r="N94" s="33"/>
       <c r="P94" s="29"/>
       <c r="Q94" s="32"/>
-      <c r="R94" s="40"/>
+      <c r="R94" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="95" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A95" s="35" t="s">
-        <v>1068</v>
+      <c r="A95" s="19" t="s">
+        <v>823</v>
       </c>
       <c r="B95" s="43" t="s">
-        <v>1070</v>
-      </c>
-      <c r="C95" s="76" t="s">
+        <v>825</v>
+      </c>
+      <c r="C95" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D95" s="66" t="s">
-        <v>1071</v>
-      </c>
-      <c r="E95" s="43" t="s">
-        <v>1070</v>
-      </c>
-      <c r="G95" s="77"/>
-      <c r="H95" s="66" t="s">
-        <v>1071</v>
-      </c>
-      <c r="I95" s="43" t="s">
-        <v>1069</v>
+      <c r="D95" s="21" t="s">
+        <v>824</v>
+      </c>
+      <c r="E95" s="26" t="s">
+        <v>825</v>
+      </c>
+      <c r="G95" s="29"/>
+      <c r="H95" s="23" t="s">
+        <v>824</v>
+      </c>
+      <c r="I95" s="26" t="s">
+        <v>826</v>
       </c>
       <c r="K95" s="29"/>
       <c r="L95" s="31"/>
@@ -7356,42 +7493,66 @@
       <c r="N95" s="33"/>
       <c r="P95" s="29"/>
       <c r="Q95" s="32"/>
-      <c r="R95" s="40"/>
+      <c r="R95" s="34" t="s">
+        <v>827</v>
+      </c>
     </row>
     <row r="96" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A96" s="35" t="s">
-        <v>1081</v>
-      </c>
-      <c r="B96" s="35"/>
-      <c r="C96" s="76"/>
-      <c r="D96" s="66" t="s">
-        <v>1083</v>
-      </c>
-      <c r="E96" s="43"/>
-      <c r="G96" s="77"/>
-      <c r="H96" s="66"/>
-      <c r="I96" s="43"/>
+      <c r="A96" s="19" t="s">
+        <v>828</v>
+      </c>
+      <c r="B96" s="43" t="s">
+        <v>830</v>
+      </c>
+      <c r="C96" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D96" s="21" t="s">
+        <v>829</v>
+      </c>
+      <c r="E96" s="26" t="s">
+        <v>830</v>
+      </c>
+      <c r="G96" s="29"/>
+      <c r="H96" s="23" t="s">
+        <v>829</v>
+      </c>
+      <c r="I96" s="26" t="s">
+        <v>831</v>
+      </c>
       <c r="K96" s="29"/>
       <c r="L96" s="31"/>
       <c r="M96" s="29"/>
       <c r="N96" s="33"/>
       <c r="P96" s="29"/>
       <c r="Q96" s="32"/>
-      <c r="R96" s="40"/>
+      <c r="R96" s="34" t="s">
+        <v>832</v>
+      </c>
     </row>
     <row r="97" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A97" s="35" t="s">
-        <v>1082</v>
-      </c>
-      <c r="B97" s="35"/>
-      <c r="C97" s="76"/>
-      <c r="D97" s="66" t="s">
-        <v>1084</v>
-      </c>
-      <c r="E97" s="43"/>
+      <c r="A97" s="65" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B97" s="43" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C97" s="76" t="s">
+        <v>20</v>
+      </c>
+      <c r="D97" s="21" t="s">
+        <v>1077</v>
+      </c>
+      <c r="E97" s="43" t="s">
+        <v>1078</v>
+      </c>
       <c r="G97" s="77"/>
-      <c r="H97" s="66"/>
-      <c r="I97" s="43"/>
+      <c r="H97" s="21" t="s">
+        <v>1077</v>
+      </c>
+      <c r="I97" s="43" t="s">
+        <v>1079</v>
+      </c>
       <c r="K97" s="29"/>
       <c r="L97" s="31"/>
       <c r="M97" s="29"/>
@@ -7402,24 +7563,26 @@
     </row>
     <row r="98" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A98" s="35" t="s">
-        <v>1085</v>
+        <v>1061</v>
       </c>
       <c r="B98" s="43" t="s">
-        <v>1088</v>
-      </c>
-      <c r="C98" s="76"/>
-      <c r="D98" s="66" t="s">
-        <v>1087</v>
+        <v>1064</v>
+      </c>
+      <c r="C98" s="76" t="s">
+        <v>20</v>
+      </c>
+      <c r="D98" s="21" t="s">
+        <v>1063</v>
       </c>
       <c r="E98" s="43" t="s">
-        <v>1088</v>
+        <v>1064</v>
       </c>
       <c r="G98" s="77"/>
-      <c r="H98" s="66" t="s">
-        <v>1087</v>
+      <c r="H98" s="21" t="s">
+        <v>1063</v>
       </c>
       <c r="I98" s="43" t="s">
-        <v>1089</v>
+        <v>1080</v>
       </c>
       <c r="K98" s="29"/>
       <c r="L98" s="31"/>
@@ -7431,24 +7594,26 @@
     </row>
     <row r="99" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A99" s="35" t="s">
-        <v>1086</v>
+        <v>1062</v>
       </c>
       <c r="B99" s="43" t="s">
-        <v>1092</v>
-      </c>
-      <c r="C99" s="76"/>
+        <v>1067</v>
+      </c>
+      <c r="C99" s="76" t="s">
+        <v>20</v>
+      </c>
       <c r="D99" s="21" t="s">
-        <v>1091</v>
+        <v>1065</v>
       </c>
       <c r="E99" s="43" t="s">
-        <v>1092</v>
+        <v>1067</v>
       </c>
       <c r="G99" s="77"/>
       <c r="H99" s="21" t="s">
-        <v>1091</v>
+        <v>1065</v>
       </c>
       <c r="I99" s="43" t="s">
-        <v>1090</v>
+        <v>1066</v>
       </c>
       <c r="K99" s="29"/>
       <c r="L99" s="31"/>
@@ -7460,24 +7625,26 @@
     </row>
     <row r="100" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A100" s="35" t="s">
-        <v>1095</v>
+        <v>1068</v>
       </c>
       <c r="B100" s="43" t="s">
-        <v>1109</v>
-      </c>
-      <c r="C100" s="76"/>
+        <v>1070</v>
+      </c>
+      <c r="C100" s="76" t="s">
+        <v>20</v>
+      </c>
       <c r="D100" s="66" t="s">
-        <v>1108</v>
+        <v>1071</v>
       </c>
       <c r="E100" s="43" t="s">
-        <v>1109</v>
+        <v>1070</v>
       </c>
       <c r="G100" s="77"/>
       <c r="H100" s="66" t="s">
-        <v>1108</v>
-      </c>
-      <c r="I100" s="68" t="s">
-        <v>1110</v>
+        <v>1071</v>
+      </c>
+      <c r="I100" s="43" t="s">
+        <v>1069</v>
       </c>
       <c r="K100" s="29"/>
       <c r="L100" s="31"/>
@@ -7489,25 +7656,17 @@
     </row>
     <row r="101" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A101" s="35" t="s">
-        <v>1100</v>
-      </c>
-      <c r="B101" s="43" t="s">
-        <v>1102</v>
-      </c>
+        <v>1081</v>
+      </c>
+      <c r="B101" s="35"/>
       <c r="C101" s="76"/>
       <c r="D101" s="66" t="s">
-        <v>1101</v>
-      </c>
-      <c r="E101" s="43" t="s">
-        <v>1102</v>
-      </c>
+        <v>1083</v>
+      </c>
+      <c r="E101" s="43"/>
       <c r="G101" s="77"/>
-      <c r="H101" s="66" t="s">
-        <v>1112</v>
-      </c>
-      <c r="I101" s="68" t="s">
-        <v>1111</v>
-      </c>
+      <c r="H101" s="66"/>
+      <c r="I101" s="43"/>
       <c r="K101" s="29"/>
       <c r="L101" s="31"/>
       <c r="M101" s="29"/>
@@ -7518,27 +7677,17 @@
     </row>
     <row r="102" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A102" s="35" t="s">
-        <v>1117</v>
-      </c>
-      <c r="B102" s="68" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C102" s="75" t="s">
-        <v>1119</v>
-      </c>
+        <v>1082</v>
+      </c>
+      <c r="B102" s="35"/>
+      <c r="C102" s="76"/>
       <c r="D102" s="66" t="s">
-        <v>1120</v>
-      </c>
-      <c r="E102" s="68" t="s">
-        <v>1121</v>
-      </c>
+        <v>1084</v>
+      </c>
+      <c r="E102" s="43"/>
       <c r="G102" s="77"/>
-      <c r="H102" s="66" t="s">
-        <v>1120</v>
-      </c>
-      <c r="I102" s="68" t="s">
-        <v>1122</v>
-      </c>
+      <c r="H102" s="66"/>
+      <c r="I102" s="43"/>
       <c r="K102" s="29"/>
       <c r="L102" s="31"/>
       <c r="M102" s="29"/>
@@ -7549,24 +7698,24 @@
     </row>
     <row r="103" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A103" s="35" t="s">
-        <v>1118</v>
-      </c>
-      <c r="B103" s="68" t="s">
-        <v>821</v>
+        <v>1085</v>
+      </c>
+      <c r="B103" s="43" t="s">
+        <v>1088</v>
       </c>
       <c r="C103" s="76"/>
       <c r="D103" s="66" t="s">
-        <v>820</v>
-      </c>
-      <c r="E103" s="68" t="s">
-        <v>821</v>
+        <v>1087</v>
+      </c>
+      <c r="E103" s="43" t="s">
+        <v>1088</v>
       </c>
       <c r="G103" s="77"/>
       <c r="H103" s="66" t="s">
-        <v>820</v>
-      </c>
-      <c r="I103" s="68" t="s">
-        <v>1124</v>
+        <v>1087</v>
+      </c>
+      <c r="I103" s="43" t="s">
+        <v>1089</v>
       </c>
       <c r="K103" s="29"/>
       <c r="L103" s="31"/>
@@ -7578,26 +7727,24 @@
     </row>
     <row r="104" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A104" s="35" t="s">
-        <v>1123</v>
-      </c>
-      <c r="B104" s="68" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C104" s="75" t="s">
-        <v>1125</v>
-      </c>
-      <c r="D104" s="66" t="s">
-        <v>1126</v>
-      </c>
-      <c r="E104" s="68" t="s">
-        <v>1127</v>
+        <v>1086</v>
+      </c>
+      <c r="B104" s="43" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C104" s="76"/>
+      <c r="D104" s="21" t="s">
+        <v>1091</v>
+      </c>
+      <c r="E104" s="43" t="s">
+        <v>1092</v>
       </c>
       <c r="G104" s="77"/>
-      <c r="H104" s="66" t="s">
-        <v>1126</v>
-      </c>
-      <c r="I104" s="68" t="s">
-        <v>1128</v>
+      <c r="H104" s="21" t="s">
+        <v>1091</v>
+      </c>
+      <c r="I104" s="43" t="s">
+        <v>1090</v>
       </c>
       <c r="K104" s="29"/>
       <c r="L104" s="31"/>
@@ -7609,24 +7756,24 @@
     </row>
     <row r="105" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A105" s="35" t="s">
-        <v>1141</v>
-      </c>
-      <c r="B105" s="68" t="s">
-        <v>1146</v>
-      </c>
-      <c r="C105" s="75"/>
+        <v>1095</v>
+      </c>
+      <c r="B105" s="43" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C105" s="76"/>
       <c r="D105" s="66" t="s">
-        <v>1147</v>
-      </c>
-      <c r="E105" s="68" t="s">
-        <v>1146</v>
+        <v>1108</v>
+      </c>
+      <c r="E105" s="43" t="s">
+        <v>1109</v>
       </c>
       <c r="G105" s="77"/>
       <c r="H105" s="66" t="s">
-        <v>1147</v>
+        <v>1108</v>
       </c>
       <c r="I105" s="68" t="s">
-        <v>1148</v>
+        <v>1110</v>
       </c>
       <c r="K105" s="29"/>
       <c r="L105" s="31"/>
@@ -7638,24 +7785,24 @@
     </row>
     <row r="106" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A106" s="35" t="s">
-        <v>1149</v>
-      </c>
-      <c r="B106" s="65" t="s">
-        <v>1151</v>
-      </c>
-      <c r="C106" s="75"/>
+        <v>1100</v>
+      </c>
+      <c r="B106" s="43" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C106" s="76"/>
       <c r="D106" s="66" t="s">
-        <v>1150</v>
-      </c>
-      <c r="E106" s="68" t="s">
-        <v>1151</v>
+        <v>1101</v>
+      </c>
+      <c r="E106" s="43" t="s">
+        <v>1102</v>
       </c>
       <c r="G106" s="77"/>
       <c r="H106" s="66" t="s">
-        <v>1150</v>
+        <v>1112</v>
       </c>
       <c r="I106" s="68" t="s">
-        <v>1152</v>
+        <v>1111</v>
       </c>
       <c r="K106" s="29"/>
       <c r="L106" s="31"/>
@@ -7667,24 +7814,26 @@
     </row>
     <row r="107" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A107" s="35" t="s">
-        <v>1158</v>
-      </c>
-      <c r="B107" s="65" t="s">
-        <v>1159</v>
-      </c>
-      <c r="C107" s="75"/>
+        <v>1117</v>
+      </c>
+      <c r="B107" s="68" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C107" s="75" t="s">
+        <v>1119</v>
+      </c>
       <c r="D107" s="66" t="s">
-        <v>1157</v>
+        <v>1120</v>
       </c>
       <c r="E107" s="68" t="s">
-        <v>1180</v>
+        <v>1121</v>
       </c>
       <c r="G107" s="77"/>
       <c r="H107" s="66" t="s">
-        <v>1157</v>
+        <v>1120</v>
       </c>
       <c r="I107" s="68" t="s">
-        <v>1160</v>
+        <v>1122</v>
       </c>
       <c r="K107" s="29"/>
       <c r="L107" s="31"/>
@@ -7696,26 +7845,24 @@
     </row>
     <row r="108" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A108" s="35" t="s">
-        <v>1169</v>
-      </c>
-      <c r="B108" s="65" t="s">
-        <v>1179</v>
-      </c>
-      <c r="C108" s="75" t="s">
-        <v>1218</v>
-      </c>
+        <v>1118</v>
+      </c>
+      <c r="B108" s="68" t="s">
+        <v>821</v>
+      </c>
+      <c r="C108" s="76"/>
       <c r="D108" s="66" t="s">
-        <v>1178</v>
+        <v>820</v>
       </c>
       <c r="E108" s="68" t="s">
-        <v>1179</v>
+        <v>821</v>
       </c>
       <c r="G108" s="77"/>
       <c r="H108" s="66" t="s">
-        <v>1178</v>
+        <v>820</v>
       </c>
       <c r="I108" s="68" t="s">
-        <v>1181</v>
+        <v>1124</v>
       </c>
       <c r="K108" s="29"/>
       <c r="L108" s="31"/>
@@ -7727,26 +7874,26 @@
     </row>
     <row r="109" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A109" s="35" t="s">
-        <v>1170</v>
-      </c>
-      <c r="B109" s="65" t="s">
-        <v>1183</v>
+        <v>1123</v>
+      </c>
+      <c r="B109" s="68" t="s">
+        <v>1127</v>
       </c>
       <c r="C109" s="75" t="s">
-        <v>1217</v>
+        <v>1125</v>
       </c>
       <c r="D109" s="66" t="s">
-        <v>1182</v>
+        <v>1126</v>
       </c>
       <c r="E109" s="68" t="s">
-        <v>1183</v>
+        <v>1127</v>
       </c>
       <c r="G109" s="77"/>
       <c r="H109" s="66" t="s">
-        <v>1182</v>
+        <v>1126</v>
       </c>
       <c r="I109" s="68" t="s">
-        <v>1184</v>
+        <v>1128</v>
       </c>
       <c r="K109" s="29"/>
       <c r="L109" s="31"/>
@@ -7758,26 +7905,24 @@
     </row>
     <row r="110" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A110" s="35" t="s">
-        <v>1171</v>
-      </c>
-      <c r="B110" s="65" t="s">
-        <v>1186</v>
-      </c>
-      <c r="C110" s="75" t="s">
-        <v>1216</v>
-      </c>
+        <v>1141</v>
+      </c>
+      <c r="B110" s="68" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C110" s="75"/>
       <c r="D110" s="66" t="s">
-        <v>1185</v>
+        <v>1147</v>
       </c>
       <c r="E110" s="68" t="s">
-        <v>1186</v>
+        <v>1146</v>
       </c>
       <c r="G110" s="77"/>
       <c r="H110" s="66" t="s">
-        <v>1185</v>
+        <v>1147</v>
       </c>
       <c r="I110" s="68" t="s">
-        <v>1187</v>
+        <v>1148</v>
       </c>
       <c r="K110" s="29"/>
       <c r="L110" s="31"/>
@@ -7789,26 +7934,24 @@
     </row>
     <row r="111" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A111" s="35" t="s">
-        <v>1172</v>
+        <v>1149</v>
       </c>
       <c r="B111" s="65" t="s">
-        <v>1189</v>
-      </c>
-      <c r="C111" s="75" t="s">
-        <v>1215</v>
-      </c>
+        <v>1151</v>
+      </c>
+      <c r="C111" s="75"/>
       <c r="D111" s="66" t="s">
-        <v>1188</v>
+        <v>1150</v>
       </c>
       <c r="E111" s="68" t="s">
-        <v>1189</v>
+        <v>1151</v>
       </c>
       <c r="G111" s="77"/>
       <c r="H111" s="66" t="s">
-        <v>1188</v>
+        <v>1150</v>
       </c>
       <c r="I111" s="68" t="s">
-        <v>1190</v>
+        <v>1152</v>
       </c>
       <c r="K111" s="29"/>
       <c r="L111" s="31"/>
@@ -7820,26 +7963,24 @@
     </row>
     <row r="112" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A112" s="35" t="s">
-        <v>1173</v>
+        <v>1158</v>
       </c>
       <c r="B112" s="65" t="s">
-        <v>1192</v>
-      </c>
-      <c r="C112" s="75" t="s">
-        <v>1214</v>
-      </c>
+        <v>1159</v>
+      </c>
+      <c r="C112" s="75"/>
       <c r="D112" s="66" t="s">
-        <v>1191</v>
+        <v>1157</v>
       </c>
       <c r="E112" s="68" t="s">
-        <v>1192</v>
+        <v>1180</v>
       </c>
       <c r="G112" s="77"/>
       <c r="H112" s="66" t="s">
-        <v>1191</v>
+        <v>1157</v>
       </c>
       <c r="I112" s="68" t="s">
-        <v>1193</v>
+        <v>1160</v>
       </c>
       <c r="K112" s="29"/>
       <c r="L112" s="31"/>
@@ -7851,26 +7992,26 @@
     </row>
     <row r="113" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A113" s="35" t="s">
-        <v>1174</v>
+        <v>1169</v>
       </c>
       <c r="B113" s="65" t="s">
-        <v>1195</v>
+        <v>1179</v>
       </c>
       <c r="C113" s="75" t="s">
-        <v>1213</v>
+        <v>1218</v>
       </c>
       <c r="D113" s="66" t="s">
-        <v>1194</v>
+        <v>1178</v>
       </c>
       <c r="E113" s="68" t="s">
-        <v>1195</v>
+        <v>1179</v>
       </c>
       <c r="G113" s="77"/>
       <c r="H113" s="66" t="s">
-        <v>1194</v>
+        <v>1178</v>
       </c>
       <c r="I113" s="68" t="s">
-        <v>1196</v>
+        <v>1181</v>
       </c>
       <c r="K113" s="29"/>
       <c r="L113" s="31"/>
@@ -7882,26 +8023,26 @@
     </row>
     <row r="114" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A114" s="35" t="s">
-        <v>1175</v>
+        <v>1170</v>
       </c>
       <c r="B114" s="65" t="s">
-        <v>1198</v>
+        <v>1183</v>
       </c>
       <c r="C114" s="75" t="s">
-        <v>203</v>
+        <v>1217</v>
       </c>
       <c r="D114" s="66" t="s">
-        <v>1197</v>
+        <v>1182</v>
       </c>
       <c r="E114" s="68" t="s">
-        <v>1198</v>
+        <v>1183</v>
       </c>
       <c r="G114" s="77"/>
       <c r="H114" s="66" t="s">
-        <v>1197</v>
+        <v>1182</v>
       </c>
       <c r="I114" s="68" t="s">
-        <v>1199</v>
+        <v>1184</v>
       </c>
       <c r="K114" s="29"/>
       <c r="L114" s="31"/>
@@ -7913,26 +8054,26 @@
     </row>
     <row r="115" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A115" s="35" t="s">
-        <v>1176</v>
+        <v>1171</v>
       </c>
       <c r="B115" s="65" t="s">
-        <v>1201</v>
+        <v>1186</v>
       </c>
       <c r="C115" s="75" t="s">
-        <v>1211</v>
+        <v>1216</v>
       </c>
       <c r="D115" s="66" t="s">
-        <v>1200</v>
+        <v>1185</v>
       </c>
       <c r="E115" s="68" t="s">
-        <v>1201</v>
+        <v>1186</v>
       </c>
       <c r="G115" s="77"/>
       <c r="H115" s="66" t="s">
-        <v>1200</v>
+        <v>1185</v>
       </c>
       <c r="I115" s="68" t="s">
-        <v>1202</v>
+        <v>1187</v>
       </c>
       <c r="K115" s="29"/>
       <c r="L115" s="31"/>
@@ -7944,26 +8085,26 @@
     </row>
     <row r="116" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A116" s="35" t="s">
-        <v>1177</v>
+        <v>1172</v>
       </c>
       <c r="B116" s="65" t="s">
-        <v>1204</v>
+        <v>1189</v>
       </c>
       <c r="C116" s="75" t="s">
-        <v>1212</v>
-      </c>
-      <c r="D116" s="74" t="s">
-        <v>1203</v>
+        <v>1215</v>
+      </c>
+      <c r="D116" s="66" t="s">
+        <v>1188</v>
       </c>
       <c r="E116" s="68" t="s">
-        <v>1204</v>
+        <v>1189</v>
       </c>
       <c r="G116" s="77"/>
       <c r="H116" s="66" t="s">
-        <v>1203</v>
+        <v>1188</v>
       </c>
       <c r="I116" s="68" t="s">
-        <v>1205</v>
+        <v>1190</v>
       </c>
       <c r="K116" s="29"/>
       <c r="L116" s="31"/>
@@ -7975,24 +8116,26 @@
     </row>
     <row r="117" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A117" s="35" t="s">
-        <v>1222</v>
+        <v>1173</v>
       </c>
       <c r="B117" s="65" t="s">
-        <v>1223</v>
-      </c>
-      <c r="C117" s="78"/>
-      <c r="D117" s="78" t="s">
-        <v>1221</v>
+        <v>1192</v>
+      </c>
+      <c r="C117" s="75" t="s">
+        <v>1214</v>
+      </c>
+      <c r="D117" s="66" t="s">
+        <v>1191</v>
       </c>
       <c r="E117" s="68" t="s">
-        <v>1223</v>
-      </c>
-      <c r="G117" s="29"/>
+        <v>1192</v>
+      </c>
+      <c r="G117" s="77"/>
       <c r="H117" s="66" t="s">
-        <v>1221</v>
+        <v>1191</v>
       </c>
       <c r="I117" s="68" t="s">
-        <v>1224</v>
+        <v>1193</v>
       </c>
       <c r="K117" s="29"/>
       <c r="L117" s="31"/>
@@ -8003,13 +8146,28 @@
       <c r="R117" s="40"/>
     </row>
     <row r="118" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A118" s="27"/>
-      <c r="B118" s="39"/>
-      <c r="D118" s="31"/>
-      <c r="E118" s="33"/>
-      <c r="G118" s="29"/>
-      <c r="H118" s="31"/>
-      <c r="I118" s="33"/>
+      <c r="A118" s="35" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B118" s="65" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C118" s="75" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D118" s="66" t="s">
+        <v>1194</v>
+      </c>
+      <c r="E118" s="68" t="s">
+        <v>1195</v>
+      </c>
+      <c r="G118" s="77"/>
+      <c r="H118" s="66" t="s">
+        <v>1194</v>
+      </c>
+      <c r="I118" s="68" t="s">
+        <v>1196</v>
+      </c>
       <c r="K118" s="29"/>
       <c r="L118" s="31"/>
       <c r="M118" s="29"/>
@@ -8019,27 +8177,27 @@
       <c r="R118" s="40"/>
     </row>
     <row r="119" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A119" s="19" t="s">
-        <v>833</v>
-      </c>
-      <c r="B119" s="43" t="s">
-        <v>835</v>
-      </c>
-      <c r="C119" s="21" t="s">
-        <v>834</v>
-      </c>
-      <c r="D119" s="23" t="s">
-        <v>834</v>
-      </c>
-      <c r="E119" s="26" t="s">
-        <v>835</v>
-      </c>
-      <c r="G119" s="29"/>
-      <c r="H119" s="23" t="s">
-        <v>834</v>
-      </c>
-      <c r="I119" s="26" t="s">
-        <v>836</v>
+      <c r="A119" s="35" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B119" s="65" t="s">
+        <v>1198</v>
+      </c>
+      <c r="C119" s="75" t="s">
+        <v>203</v>
+      </c>
+      <c r="D119" s="66" t="s">
+        <v>1197</v>
+      </c>
+      <c r="E119" s="68" t="s">
+        <v>1198</v>
+      </c>
+      <c r="G119" s="77"/>
+      <c r="H119" s="66" t="s">
+        <v>1197</v>
+      </c>
+      <c r="I119" s="68" t="s">
+        <v>1199</v>
       </c>
       <c r="K119" s="29"/>
       <c r="L119" s="31"/>
@@ -8047,32 +8205,30 @@
       <c r="N119" s="33"/>
       <c r="P119" s="29"/>
       <c r="Q119" s="32"/>
-      <c r="R119" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R119" s="40"/>
     </row>
     <row r="120" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A120" s="65" t="s">
-        <v>837</v>
-      </c>
-      <c r="B120" s="43" t="s">
-        <v>839</v>
-      </c>
-      <c r="C120" s="21" t="s">
-        <v>838</v>
-      </c>
-      <c r="D120" s="23" t="s">
-        <v>838</v>
-      </c>
-      <c r="E120" s="26" t="s">
-        <v>839</v>
-      </c>
-      <c r="G120" s="29"/>
-      <c r="H120" s="23" t="s">
-        <v>838</v>
-      </c>
-      <c r="I120" s="26" t="s">
-        <v>840</v>
+      <c r="A120" s="35" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B120" s="65" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C120" s="75" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D120" s="66" t="s">
+        <v>1200</v>
+      </c>
+      <c r="E120" s="68" t="s">
+        <v>1201</v>
+      </c>
+      <c r="G120" s="77"/>
+      <c r="H120" s="66" t="s">
+        <v>1200</v>
+      </c>
+      <c r="I120" s="68" t="s">
+        <v>1202</v>
       </c>
       <c r="K120" s="29"/>
       <c r="L120" s="31"/>
@@ -8080,32 +8236,30 @@
       <c r="N120" s="33"/>
       <c r="P120" s="29"/>
       <c r="Q120" s="32"/>
-      <c r="R120" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R120" s="40"/>
     </row>
     <row r="121" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A121" s="19" t="s">
-        <v>841</v>
-      </c>
-      <c r="B121" s="43" t="s">
-        <v>843</v>
-      </c>
-      <c r="C121" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D121" s="23" t="s">
-        <v>842</v>
-      </c>
-      <c r="E121" s="26" t="s">
-        <v>843</v>
-      </c>
-      <c r="G121" s="29"/>
-      <c r="H121" s="42" t="s">
-        <v>842</v>
-      </c>
-      <c r="I121" s="26" t="s">
-        <v>844</v>
+      <c r="A121" s="35" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B121" s="65" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C121" s="75" t="s">
+        <v>1212</v>
+      </c>
+      <c r="D121" s="74" t="s">
+        <v>1203</v>
+      </c>
+      <c r="E121" s="68" t="s">
+        <v>1204</v>
+      </c>
+      <c r="G121" s="77"/>
+      <c r="H121" s="66" t="s">
+        <v>1203</v>
+      </c>
+      <c r="I121" s="68" t="s">
+        <v>1205</v>
       </c>
       <c r="K121" s="29"/>
       <c r="L121" s="31"/>
@@ -8113,32 +8267,28 @@
       <c r="N121" s="33"/>
       <c r="P121" s="29"/>
       <c r="Q121" s="32"/>
-      <c r="R121" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R121" s="40"/>
     </row>
     <row r="122" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A122" s="19" t="s">
-        <v>845</v>
-      </c>
-      <c r="B122" s="43" t="s">
-        <v>847</v>
-      </c>
-      <c r="C122" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D122" s="23" t="s">
-        <v>846</v>
-      </c>
-      <c r="E122" s="26" t="s">
-        <v>847</v>
+      <c r="A122" s="35" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B122" s="65" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C122" s="78"/>
+      <c r="D122" s="78" t="s">
+        <v>1221</v>
+      </c>
+      <c r="E122" s="68" t="s">
+        <v>1223</v>
       </c>
       <c r="G122" s="29"/>
-      <c r="H122" s="42" t="s">
-        <v>846</v>
-      </c>
-      <c r="I122" s="26" t="s">
-        <v>848</v>
+      <c r="H122" s="66" t="s">
+        <v>1221</v>
+      </c>
+      <c r="I122" s="68" t="s">
+        <v>1224</v>
       </c>
       <c r="K122" s="29"/>
       <c r="L122" s="31"/>
@@ -8146,63 +8296,46 @@
       <c r="N122" s="33"/>
       <c r="P122" s="29"/>
       <c r="Q122" s="32"/>
-      <c r="R122" s="34" t="s">
-        <v>849</v>
-      </c>
+      <c r="R122" s="40"/>
     </row>
     <row r="123" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A123" s="19" t="s">
-        <v>850</v>
-      </c>
-      <c r="B123" s="43" t="s">
-        <v>852</v>
-      </c>
-      <c r="C123" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D123" s="23" t="s">
-        <v>851</v>
-      </c>
-      <c r="E123" s="26" t="s">
-        <v>852</v>
-      </c>
+      <c r="A123" s="27"/>
+      <c r="B123" s="39"/>
+      <c r="D123" s="31"/>
+      <c r="E123" s="33"/>
       <c r="G123" s="29"/>
-      <c r="H123" s="42" t="s">
-        <v>851</v>
-      </c>
-      <c r="I123" s="26" t="s">
-        <v>853</v>
-      </c>
+      <c r="H123" s="31"/>
+      <c r="I123" s="33"/>
       <c r="K123" s="29"/>
       <c r="L123" s="31"/>
       <c r="M123" s="29"/>
       <c r="N123" s="33"/>
       <c r="P123" s="29"/>
       <c r="Q123" s="32"/>
-      <c r="R123" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R123" s="40"/>
     </row>
     <row r="124" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A124" s="35" t="s">
-        <v>1093</v>
-      </c>
-      <c r="B124" s="68" t="s">
-        <v>1113</v>
-      </c>
-      <c r="C124" s="21"/>
-      <c r="D124" s="67" t="s">
-        <v>1094</v>
-      </c>
-      <c r="E124" s="68" t="s">
-        <v>1113</v>
+      <c r="A124" s="19" t="s">
+        <v>833</v>
+      </c>
+      <c r="B124" s="43" t="s">
+        <v>835</v>
+      </c>
+      <c r="C124" s="21" t="s">
+        <v>834</v>
+      </c>
+      <c r="D124" s="23" t="s">
+        <v>834</v>
+      </c>
+      <c r="E124" s="26" t="s">
+        <v>835</v>
       </c>
       <c r="G124" s="29"/>
-      <c r="H124" s="67" t="s">
-        <v>1094</v>
-      </c>
-      <c r="I124" s="43" t="s">
-        <v>1114</v>
+      <c r="H124" s="23" t="s">
+        <v>834</v>
+      </c>
+      <c r="I124" s="26" t="s">
+        <v>836</v>
       </c>
       <c r="K124" s="29"/>
       <c r="L124" s="31"/>
@@ -8210,28 +8343,32 @@
       <c r="N124" s="33"/>
       <c r="P124" s="29"/>
       <c r="Q124" s="32"/>
-      <c r="R124" s="40"/>
+      <c r="R124" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="125" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A125" s="35" t="s">
-        <v>1096</v>
+      <c r="A125" s="65" t="s">
+        <v>837</v>
       </c>
       <c r="B125" s="43" t="s">
-        <v>1098</v>
-      </c>
-      <c r="C125" s="21"/>
-      <c r="D125" s="42" t="s">
-        <v>1097</v>
-      </c>
-      <c r="E125" s="43" t="s">
-        <v>1098</v>
+        <v>839</v>
+      </c>
+      <c r="C125" s="21" t="s">
+        <v>838</v>
+      </c>
+      <c r="D125" s="23" t="s">
+        <v>838</v>
+      </c>
+      <c r="E125" s="26" t="s">
+        <v>839</v>
       </c>
       <c r="G125" s="29"/>
-      <c r="H125" s="42" t="s">
-        <v>1097</v>
-      </c>
-      <c r="I125" s="43" t="s">
-        <v>1099</v>
+      <c r="H125" s="23" t="s">
+        <v>838</v>
+      </c>
+      <c r="I125" s="26" t="s">
+        <v>840</v>
       </c>
       <c r="K125" s="29"/>
       <c r="L125" s="31"/>
@@ -8239,28 +8376,32 @@
       <c r="N125" s="33"/>
       <c r="P125" s="29"/>
       <c r="Q125" s="32"/>
-      <c r="R125" s="40"/>
+      <c r="R125" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="126" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A126" s="35" t="s">
-        <v>1153</v>
-      </c>
-      <c r="B126" s="35" t="s">
-        <v>1154</v>
-      </c>
-      <c r="C126" s="21"/>
-      <c r="D126" s="67" t="s">
-        <v>1155</v>
-      </c>
-      <c r="E126" s="35" t="s">
-        <v>1154</v>
+      <c r="A126" s="19" t="s">
+        <v>841</v>
+      </c>
+      <c r="B126" s="43" t="s">
+        <v>843</v>
+      </c>
+      <c r="C126" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D126" s="23" t="s">
+        <v>842</v>
+      </c>
+      <c r="E126" s="26" t="s">
+        <v>843</v>
       </c>
       <c r="G126" s="29"/>
       <c r="H126" s="42" t="s">
-        <v>1155</v>
-      </c>
-      <c r="I126" s="43" t="s">
-        <v>1156</v>
+        <v>842</v>
+      </c>
+      <c r="I126" s="26" t="s">
+        <v>844</v>
       </c>
       <c r="K126" s="29"/>
       <c r="L126" s="31"/>
@@ -8268,46 +8409,65 @@
       <c r="N126" s="33"/>
       <c r="P126" s="29"/>
       <c r="Q126" s="32"/>
-      <c r="R126" s="40"/>
+      <c r="R126" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="127" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A127" s="27"/>
-      <c r="B127" s="39"/>
-      <c r="D127" s="31"/>
-      <c r="E127" s="33"/>
+      <c r="A127" s="19" t="s">
+        <v>845</v>
+      </c>
+      <c r="B127" s="43" t="s">
+        <v>847</v>
+      </c>
+      <c r="C127" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D127" s="23" t="s">
+        <v>846</v>
+      </c>
+      <c r="E127" s="26" t="s">
+        <v>847</v>
+      </c>
       <c r="G127" s="29"/>
-      <c r="H127" s="31"/>
-      <c r="I127" s="33"/>
+      <c r="H127" s="42" t="s">
+        <v>846</v>
+      </c>
+      <c r="I127" s="26" t="s">
+        <v>848</v>
+      </c>
       <c r="K127" s="29"/>
       <c r="L127" s="31"/>
       <c r="M127" s="29"/>
       <c r="N127" s="33"/>
       <c r="P127" s="29"/>
       <c r="Q127" s="32"/>
-      <c r="R127" s="34"/>
+      <c r="R127" s="34" t="s">
+        <v>849</v>
+      </c>
     </row>
     <row r="128" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A128" s="19" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="B128" s="43" t="s">
-        <v>857</v>
+        <v>852</v>
       </c>
       <c r="C128" s="21" t="s">
-        <v>855</v>
+        <v>20</v>
       </c>
       <c r="D128" s="23" t="s">
-        <v>20</v>
+        <v>851</v>
       </c>
       <c r="E128" s="26" t="s">
-        <v>20</v>
+        <v>852</v>
       </c>
       <c r="G128" s="29"/>
-      <c r="H128" s="23" t="s">
-        <v>856</v>
+      <c r="H128" s="42" t="s">
+        <v>851</v>
       </c>
       <c r="I128" s="26" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="K128" s="29"/>
       <c r="L128" s="31"/>
@@ -8315,29 +8475,30 @@
       <c r="N128" s="33"/>
       <c r="P128" s="29"/>
       <c r="Q128" s="32"/>
-      <c r="R128" s="34" t="s">
-        <v>849</v>
+      <c r="R128" s="34" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A129" s="35" t="s">
-        <v>1165</v>
-      </c>
-      <c r="B129" s="33" t="s">
-        <v>1166</v>
-      </c>
-      <c r="D129" s="70" t="s">
-        <v>1167</v>
-      </c>
-      <c r="E129" s="33" t="s">
-        <v>1166</v>
+        <v>1093</v>
+      </c>
+      <c r="B129" s="68" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C129" s="21"/>
+      <c r="D129" s="67" t="s">
+        <v>1094</v>
+      </c>
+      <c r="E129" s="68" t="s">
+        <v>1113</v>
       </c>
       <c r="G129" s="29"/>
-      <c r="H129" s="70" t="s">
-        <v>1167</v>
-      </c>
-      <c r="I129" s="33" t="s">
-        <v>1168</v>
+      <c r="H129" s="67" t="s">
+        <v>1094</v>
+      </c>
+      <c r="I129" s="43" t="s">
+        <v>1114</v>
       </c>
       <c r="K129" s="29"/>
       <c r="L129" s="31"/>
@@ -8348,14 +8509,26 @@
       <c r="R129" s="40"/>
     </row>
     <row r="130" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A130" s="19"/>
-      <c r="B130" s="39"/>
+      <c r="A130" s="35" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B130" s="43" t="s">
+        <v>1098</v>
+      </c>
       <c r="C130" s="21"/>
-      <c r="D130" s="31"/>
-      <c r="E130" s="33"/>
+      <c r="D130" s="42" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E130" s="43" t="s">
+        <v>1098</v>
+      </c>
       <c r="G130" s="29"/>
-      <c r="H130" s="31"/>
-      <c r="I130" s="33"/>
+      <c r="H130" s="42" t="s">
+        <v>1097</v>
+      </c>
+      <c r="I130" s="43" t="s">
+        <v>1099</v>
+      </c>
       <c r="K130" s="29"/>
       <c r="L130" s="31"/>
       <c r="M130" s="29"/>
@@ -8365,27 +8538,25 @@
       <c r="R130" s="40"/>
     </row>
     <row r="131" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A131" s="65" t="s">
-        <v>858</v>
-      </c>
-      <c r="B131" s="43" t="s">
-        <v>860</v>
-      </c>
-      <c r="C131" s="19" t="s">
-        <v>859</v>
-      </c>
-      <c r="D131" s="21" t="s">
-        <v>859</v>
-      </c>
-      <c r="E131" s="26" t="s">
-        <v>860</v>
-      </c>
-      <c r="G131" s="33"/>
-      <c r="H131" s="21" t="s">
-        <v>859</v>
-      </c>
-      <c r="I131" s="26" t="s">
-        <v>861</v>
+      <c r="A131" s="35" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B131" s="35" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C131" s="21"/>
+      <c r="D131" s="67" t="s">
+        <v>1155</v>
+      </c>
+      <c r="E131" s="35" t="s">
+        <v>1154</v>
+      </c>
+      <c r="G131" s="29"/>
+      <c r="H131" s="42" t="s">
+        <v>1155</v>
+      </c>
+      <c r="I131" s="43" t="s">
+        <v>1156</v>
       </c>
       <c r="K131" s="29"/>
       <c r="L131" s="31"/>
@@ -8393,63 +8564,46 @@
       <c r="N131" s="33"/>
       <c r="P131" s="29"/>
       <c r="Q131" s="32"/>
-      <c r="R131" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R131" s="40"/>
     </row>
     <row r="132" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A132" s="19" t="s">
-        <v>862</v>
-      </c>
-      <c r="B132" s="43" t="s">
-        <v>864</v>
-      </c>
-      <c r="C132" s="21" t="s">
-        <v>863</v>
-      </c>
-      <c r="D132" s="23" t="s">
-        <v>863</v>
-      </c>
-      <c r="E132" s="26" t="s">
-        <v>864</v>
-      </c>
+      <c r="A132" s="27"/>
+      <c r="B132" s="39"/>
+      <c r="D132" s="31"/>
+      <c r="E132" s="33"/>
       <c r="G132" s="29"/>
-      <c r="H132" s="23" t="s">
-        <v>863</v>
-      </c>
-      <c r="I132" s="26" t="s">
-        <v>865</v>
-      </c>
+      <c r="H132" s="31"/>
+      <c r="I132" s="33"/>
       <c r="K132" s="29"/>
       <c r="L132" s="31"/>
       <c r="M132" s="29"/>
       <c r="N132" s="33"/>
       <c r="P132" s="29"/>
       <c r="Q132" s="32"/>
-      <c r="R132" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R132" s="34"/>
     </row>
     <row r="133" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A133" s="65" t="s">
-        <v>1145</v>
-      </c>
-      <c r="B133" s="68" t="s">
-        <v>1143</v>
-      </c>
-      <c r="C133" s="75"/>
-      <c r="D133" s="66" t="s">
-        <v>1142</v>
-      </c>
-      <c r="E133" s="68" t="s">
-        <v>1143</v>
-      </c>
-      <c r="G133" s="77"/>
-      <c r="H133" s="66" t="s">
-        <v>1142</v>
-      </c>
-      <c r="I133" s="68" t="s">
-        <v>1144</v>
+      <c r="A133" s="19" t="s">
+        <v>854</v>
+      </c>
+      <c r="B133" s="43" t="s">
+        <v>857</v>
+      </c>
+      <c r="C133" s="21" t="s">
+        <v>855</v>
+      </c>
+      <c r="D133" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E133" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G133" s="29"/>
+      <c r="H133" s="23" t="s">
+        <v>856</v>
+      </c>
+      <c r="I133" s="26" t="s">
+        <v>857</v>
       </c>
       <c r="K133" s="29"/>
       <c r="L133" s="31"/>
@@ -8457,16 +8611,30 @@
       <c r="N133" s="33"/>
       <c r="P133" s="29"/>
       <c r="Q133" s="32"/>
-      <c r="R133" s="40"/>
+      <c r="R133" s="34" t="s">
+        <v>849</v>
+      </c>
     </row>
     <row r="134" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A134" s="27"/>
-      <c r="B134" s="39"/>
-      <c r="D134" s="31"/>
-      <c r="E134" s="33"/>
+      <c r="A134" s="35" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B134" s="33" t="s">
+        <v>1166</v>
+      </c>
+      <c r="D134" s="70" t="s">
+        <v>1167</v>
+      </c>
+      <c r="E134" s="33" t="s">
+        <v>1166</v>
+      </c>
       <c r="G134" s="29"/>
-      <c r="H134" s="31"/>
-      <c r="I134" s="33"/>
+      <c r="H134" s="70" t="s">
+        <v>1167</v>
+      </c>
+      <c r="I134" s="33" t="s">
+        <v>1168</v>
+      </c>
       <c r="K134" s="29"/>
       <c r="L134" s="31"/>
       <c r="M134" s="29"/>
@@ -8476,60 +8644,44 @@
       <c r="R134" s="40"/>
     </row>
     <row r="135" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A135" s="19" t="s">
-        <v>866</v>
-      </c>
-      <c r="B135" s="43" t="s">
-        <v>868</v>
-      </c>
-      <c r="C135" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D135" s="23" t="s">
-        <v>867</v>
-      </c>
-      <c r="E135" s="26" t="s">
-        <v>868</v>
-      </c>
+      <c r="A135" s="19"/>
+      <c r="B135" s="39"/>
+      <c r="C135" s="21"/>
+      <c r="D135" s="31"/>
+      <c r="E135" s="33"/>
       <c r="G135" s="29"/>
-      <c r="H135" s="23" t="s">
-        <v>867</v>
-      </c>
-      <c r="I135" s="26" t="s">
-        <v>869</v>
-      </c>
+      <c r="H135" s="31"/>
+      <c r="I135" s="33"/>
       <c r="K135" s="29"/>
       <c r="L135" s="31"/>
       <c r="M135" s="29"/>
       <c r="N135" s="33"/>
       <c r="P135" s="29"/>
       <c r="Q135" s="32"/>
-      <c r="R135" s="34" t="s">
-        <v>33</v>
-      </c>
+      <c r="R135" s="40"/>
     </row>
     <row r="136" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A136" s="19" t="s">
-        <v>870</v>
+      <c r="A136" s="65" t="s">
+        <v>858</v>
       </c>
       <c r="B136" s="43" t="s">
-        <v>872</v>
-      </c>
-      <c r="C136" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D136" s="23" t="s">
-        <v>871</v>
+        <v>860</v>
+      </c>
+      <c r="C136" s="19" t="s">
+        <v>859</v>
+      </c>
+      <c r="D136" s="21" t="s">
+        <v>859</v>
       </c>
       <c r="E136" s="26" t="s">
-        <v>872</v>
-      </c>
-      <c r="G136" s="29"/>
-      <c r="H136" s="23" t="s">
-        <v>871</v>
+        <v>860</v>
+      </c>
+      <c r="G136" s="33"/>
+      <c r="H136" s="21" t="s">
+        <v>859</v>
       </c>
       <c r="I136" s="26" t="s">
-        <v>873</v>
+        <v>861</v>
       </c>
       <c r="K136" s="29"/>
       <c r="L136" s="31"/>
@@ -8537,32 +8689,32 @@
       <c r="N136" s="33"/>
       <c r="P136" s="29"/>
       <c r="Q136" s="32"/>
-      <c r="R136" s="34" t="s">
-        <v>33</v>
+      <c r="R136" s="34" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A137" s="19" t="s">
-        <v>874</v>
+        <v>862</v>
       </c>
       <c r="B137" s="43" t="s">
-        <v>876</v>
+        <v>864</v>
       </c>
       <c r="C137" s="21" t="s">
-        <v>20</v>
+        <v>863</v>
       </c>
       <c r="D137" s="23" t="s">
-        <v>875</v>
+        <v>863</v>
       </c>
       <c r="E137" s="26" t="s">
-        <v>876</v>
+        <v>864</v>
       </c>
       <c r="G137" s="29"/>
       <c r="H137" s="23" t="s">
-        <v>875</v>
+        <v>863</v>
       </c>
       <c r="I137" s="26" t="s">
-        <v>877</v>
+        <v>865</v>
       </c>
       <c r="K137" s="29"/>
       <c r="L137" s="31"/>
@@ -8570,32 +8722,30 @@
       <c r="N137" s="33"/>
       <c r="P137" s="29"/>
       <c r="Q137" s="32"/>
-      <c r="R137" s="34" t="s">
-        <v>33</v>
+      <c r="R137" s="34" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A138" s="19" t="s">
-        <v>878</v>
-      </c>
-      <c r="B138" s="43" t="s">
-        <v>880</v>
-      </c>
-      <c r="C138" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D138" s="23" t="s">
-        <v>879</v>
-      </c>
-      <c r="E138" s="26" t="s">
-        <v>880</v>
-      </c>
-      <c r="G138" s="29"/>
-      <c r="H138" s="23" t="s">
-        <v>879</v>
-      </c>
-      <c r="I138" s="26" t="s">
-        <v>881</v>
+      <c r="A138" s="65" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B138" s="68" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C138" s="75"/>
+      <c r="D138" s="66" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E138" s="68" t="s">
+        <v>1143</v>
+      </c>
+      <c r="G138" s="77"/>
+      <c r="H138" s="66" t="s">
+        <v>1142</v>
+      </c>
+      <c r="I138" s="68" t="s">
+        <v>1144</v>
       </c>
       <c r="K138" s="29"/>
       <c r="L138" s="31"/>
@@ -8603,32 +8753,28 @@
       <c r="N138" s="33"/>
       <c r="P138" s="29"/>
       <c r="Q138" s="32"/>
-      <c r="R138" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R138" s="40"/>
     </row>
     <row r="139" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A139" s="19" t="s">
-        <v>882</v>
-      </c>
-      <c r="B139" s="43" t="s">
-        <v>884</v>
-      </c>
-      <c r="C139" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D139" s="23" t="s">
-        <v>883</v>
-      </c>
-      <c r="E139" s="26" t="s">
-        <v>884</v>
+      <c r="A139" s="65" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B139" s="65" t="s">
+        <v>1263</v>
+      </c>
+      <c r="C139" s="78"/>
+      <c r="D139" s="66" t="s">
+        <v>1262</v>
+      </c>
+      <c r="E139" s="68" t="s">
+        <v>1263</v>
       </c>
       <c r="G139" s="29"/>
-      <c r="H139" s="23" t="s">
-        <v>883</v>
-      </c>
-      <c r="I139" s="26" t="s">
-        <v>885</v>
+      <c r="H139" s="66" t="s">
+        <v>1262</v>
+      </c>
+      <c r="I139" s="68" t="s">
+        <v>1264</v>
       </c>
       <c r="K139" s="29"/>
       <c r="L139" s="31"/>
@@ -8636,32 +8782,28 @@
       <c r="N139" s="33"/>
       <c r="P139" s="29"/>
       <c r="Q139" s="32"/>
-      <c r="R139" s="34" t="s">
-        <v>33</v>
-      </c>
+      <c r="R139" s="40"/>
     </row>
     <row r="140" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A140" s="19" t="s">
-        <v>886</v>
-      </c>
-      <c r="B140" s="43" t="s">
-        <v>888</v>
-      </c>
-      <c r="C140" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D140" s="23" t="s">
-        <v>887</v>
-      </c>
-      <c r="E140" s="26" t="s">
-        <v>888</v>
+      <c r="A140" s="65" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B140" s="65" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C140" s="78"/>
+      <c r="D140" s="66" t="s">
+        <v>1265</v>
+      </c>
+      <c r="E140" s="68" t="s">
+        <v>1266</v>
       </c>
       <c r="G140" s="29"/>
-      <c r="H140" s="23" t="s">
-        <v>887</v>
-      </c>
-      <c r="I140" s="26" t="s">
-        <v>889</v>
+      <c r="H140" s="66" t="s">
+        <v>1265</v>
+      </c>
+      <c r="I140" s="68" t="s">
+        <v>1267</v>
       </c>
       <c r="K140" s="29"/>
       <c r="L140" s="31"/>
@@ -8669,32 +8811,28 @@
       <c r="N140" s="33"/>
       <c r="P140" s="29"/>
       <c r="Q140" s="32"/>
-      <c r="R140" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R140" s="40"/>
     </row>
     <row r="141" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A141" s="19" t="s">
-        <v>890</v>
-      </c>
-      <c r="B141" s="43" t="s">
-        <v>892</v>
-      </c>
-      <c r="C141" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D141" s="23" t="s">
-        <v>891</v>
-      </c>
-      <c r="E141" s="26" t="s">
-        <v>892</v>
+      <c r="A141" s="65" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B141" s="65" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C141" s="78"/>
+      <c r="D141" s="66" t="s">
+        <v>1260</v>
+      </c>
+      <c r="E141" s="68" t="s">
+        <v>1261</v>
       </c>
       <c r="G141" s="29"/>
-      <c r="H141" s="23" t="s">
-        <v>891</v>
-      </c>
-      <c r="I141" s="26" t="s">
-        <v>893</v>
+      <c r="H141" s="66" t="s">
+        <v>1260</v>
+      </c>
+      <c r="I141" s="68" t="s">
+        <v>1261</v>
       </c>
       <c r="K141" s="29"/>
       <c r="L141" s="31"/>
@@ -8702,73 +8840,79 @@
       <c r="N141" s="33"/>
       <c r="P141" s="29"/>
       <c r="Q141" s="32"/>
-      <c r="R141" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R141" s="40"/>
     </row>
     <row r="142" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A142" s="27" t="s">
-        <v>1072</v>
-      </c>
-      <c r="B142" s="69" t="s">
-        <v>1115</v>
-      </c>
-      <c r="D142" s="70" t="s">
-        <v>1073</v>
-      </c>
-      <c r="E142" s="69" t="s">
-        <v>1115</v>
-      </c>
+      <c r="A142" s="27"/>
+      <c r="B142" s="39"/>
+      <c r="D142" s="31"/>
+      <c r="E142" s="33"/>
       <c r="G142" s="29"/>
-      <c r="H142" s="70" t="s">
-        <v>1073</v>
-      </c>
-      <c r="I142" s="69" t="s">
-        <v>1116</v>
-      </c>
+      <c r="H142" s="31"/>
+      <c r="I142" s="33"/>
       <c r="K142" s="29"/>
       <c r="L142" s="31"/>
       <c r="M142" s="29"/>
       <c r="N142" s="33"/>
       <c r="P142" s="29"/>
       <c r="Q142" s="32"/>
-      <c r="R142" s="27"/>
+      <c r="R142" s="40"/>
     </row>
     <row r="143" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A143" s="27"/>
-      <c r="B143" s="39"/>
-      <c r="D143" s="31"/>
-      <c r="E143" s="33"/>
+      <c r="A143" s="19" t="s">
+        <v>866</v>
+      </c>
+      <c r="B143" s="43" t="s">
+        <v>868</v>
+      </c>
+      <c r="C143" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D143" s="23" t="s">
+        <v>867</v>
+      </c>
+      <c r="E143" s="26" t="s">
+        <v>868</v>
+      </c>
       <c r="G143" s="29"/>
-      <c r="H143" s="31"/>
-      <c r="I143" s="33"/>
+      <c r="H143" s="23" t="s">
+        <v>867</v>
+      </c>
+      <c r="I143" s="26" t="s">
+        <v>869</v>
+      </c>
       <c r="K143" s="29"/>
       <c r="L143" s="31"/>
       <c r="M143" s="29"/>
       <c r="N143" s="33"/>
       <c r="P143" s="29"/>
       <c r="Q143" s="32"/>
-      <c r="R143" s="27"/>
+      <c r="R143" s="34" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="144" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A144" s="27" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B144" s="79" t="s">
-        <v>1226</v>
-      </c>
-      <c r="D144" s="31" t="s">
-        <v>312</v>
-      </c>
-      <c r="E144" s="33" t="s">
-        <v>1226</v>
+      <c r="A144" s="19" t="s">
+        <v>870</v>
+      </c>
+      <c r="B144" s="43" t="s">
+        <v>872</v>
+      </c>
+      <c r="C144" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D144" s="23" t="s">
+        <v>871</v>
+      </c>
+      <c r="E144" s="26" t="s">
+        <v>872</v>
       </c>
       <c r="G144" s="29"/>
-      <c r="H144" s="31" t="s">
-        <v>312</v>
-      </c>
-      <c r="I144" s="33" t="s">
-        <v>1227</v>
+      <c r="H144" s="23" t="s">
+        <v>871</v>
+      </c>
+      <c r="I144" s="26" t="s">
+        <v>873</v>
       </c>
       <c r="K144" s="29"/>
       <c r="L144" s="31"/>
@@ -8776,96 +8920,195 @@
       <c r="N144" s="33"/>
       <c r="P144" s="29"/>
       <c r="Q144" s="32"/>
-      <c r="R144" s="27"/>
+      <c r="R144" s="34" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="145" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A145" s="27"/>
-      <c r="B145" s="39"/>
-      <c r="D145" s="31"/>
-      <c r="E145" s="33"/>
+      <c r="A145" s="19" t="s">
+        <v>874</v>
+      </c>
+      <c r="B145" s="43" t="s">
+        <v>876</v>
+      </c>
+      <c r="C145" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D145" s="23" t="s">
+        <v>875</v>
+      </c>
+      <c r="E145" s="26" t="s">
+        <v>876</v>
+      </c>
       <c r="G145" s="29"/>
-      <c r="H145" s="31"/>
-      <c r="I145" s="33"/>
+      <c r="H145" s="23" t="s">
+        <v>875</v>
+      </c>
+      <c r="I145" s="26" t="s">
+        <v>877</v>
+      </c>
       <c r="K145" s="29"/>
       <c r="L145" s="31"/>
       <c r="M145" s="29"/>
       <c r="N145" s="33"/>
       <c r="P145" s="29"/>
       <c r="Q145" s="32"/>
-      <c r="R145" s="27"/>
+      <c r="R145" s="34" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="146" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A146" s="27"/>
-      <c r="B146" s="39"/>
-      <c r="D146" s="31"/>
-      <c r="E146" s="33"/>
+      <c r="A146" s="19" t="s">
+        <v>878</v>
+      </c>
+      <c r="B146" s="43" t="s">
+        <v>880</v>
+      </c>
+      <c r="C146" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D146" s="23" t="s">
+        <v>879</v>
+      </c>
+      <c r="E146" s="26" t="s">
+        <v>880</v>
+      </c>
       <c r="G146" s="29"/>
-      <c r="H146" s="31"/>
-      <c r="I146" s="33"/>
+      <c r="H146" s="23" t="s">
+        <v>879</v>
+      </c>
+      <c r="I146" s="26" t="s">
+        <v>881</v>
+      </c>
       <c r="K146" s="29"/>
       <c r="L146" s="31"/>
       <c r="M146" s="29"/>
       <c r="N146" s="33"/>
       <c r="P146" s="29"/>
       <c r="Q146" s="32"/>
-      <c r="R146" s="27"/>
+      <c r="R146" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="147" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A147" s="27"/>
-      <c r="B147" s="39"/>
-      <c r="D147" s="31"/>
-      <c r="E147" s="33"/>
+      <c r="A147" s="19" t="s">
+        <v>882</v>
+      </c>
+      <c r="B147" s="43" t="s">
+        <v>884</v>
+      </c>
+      <c r="C147" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D147" s="23" t="s">
+        <v>883</v>
+      </c>
+      <c r="E147" s="26" t="s">
+        <v>884</v>
+      </c>
       <c r="G147" s="29"/>
-      <c r="H147" s="31"/>
-      <c r="I147" s="33"/>
+      <c r="H147" s="23" t="s">
+        <v>883</v>
+      </c>
+      <c r="I147" s="26" t="s">
+        <v>885</v>
+      </c>
       <c r="K147" s="29"/>
       <c r="L147" s="31"/>
       <c r="M147" s="29"/>
       <c r="N147" s="33"/>
       <c r="P147" s="29"/>
       <c r="Q147" s="32"/>
-      <c r="R147" s="27"/>
+      <c r="R147" s="34" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="148" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A148" s="27"/>
-      <c r="B148" s="39"/>
-      <c r="D148" s="31"/>
-      <c r="E148" s="33"/>
+      <c r="A148" s="19" t="s">
+        <v>886</v>
+      </c>
+      <c r="B148" s="43" t="s">
+        <v>888</v>
+      </c>
+      <c r="C148" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D148" s="23" t="s">
+        <v>887</v>
+      </c>
+      <c r="E148" s="26" t="s">
+        <v>888</v>
+      </c>
       <c r="G148" s="29"/>
-      <c r="H148" s="31"/>
-      <c r="I148" s="33"/>
+      <c r="H148" s="23" t="s">
+        <v>887</v>
+      </c>
+      <c r="I148" s="26" t="s">
+        <v>889</v>
+      </c>
       <c r="K148" s="29"/>
       <c r="L148" s="31"/>
       <c r="M148" s="29"/>
       <c r="N148" s="33"/>
       <c r="P148" s="29"/>
       <c r="Q148" s="32"/>
-      <c r="R148" s="27"/>
+      <c r="R148" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="149" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A149" s="27"/>
-      <c r="B149" s="39"/>
-      <c r="D149" s="31"/>
-      <c r="E149" s="33"/>
+      <c r="A149" s="19" t="s">
+        <v>890</v>
+      </c>
+      <c r="B149" s="43" t="s">
+        <v>892</v>
+      </c>
+      <c r="C149" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D149" s="23" t="s">
+        <v>891</v>
+      </c>
+      <c r="E149" s="26" t="s">
+        <v>892</v>
+      </c>
       <c r="G149" s="29"/>
-      <c r="H149" s="31"/>
-      <c r="I149" s="33"/>
+      <c r="H149" s="23" t="s">
+        <v>891</v>
+      </c>
+      <c r="I149" s="26" t="s">
+        <v>893</v>
+      </c>
       <c r="K149" s="29"/>
       <c r="L149" s="31"/>
       <c r="M149" s="29"/>
       <c r="N149" s="33"/>
       <c r="P149" s="29"/>
       <c r="Q149" s="32"/>
-      <c r="R149" s="27"/>
+      <c r="R149" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="150" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A150" s="27"/>
-      <c r="B150" s="39"/>
-      <c r="D150" s="31"/>
-      <c r="E150" s="33"/>
+      <c r="A150" s="27" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B150" s="69" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D150" s="70" t="s">
+        <v>1073</v>
+      </c>
+      <c r="E150" s="69" t="s">
+        <v>1115</v>
+      </c>
       <c r="G150" s="29"/>
-      <c r="H150" s="31"/>
-      <c r="I150" s="33"/>
+      <c r="H150" s="70" t="s">
+        <v>1073</v>
+      </c>
+      <c r="I150" s="69" t="s">
+        <v>1116</v>
+      </c>
       <c r="K150" s="29"/>
       <c r="L150" s="31"/>
       <c r="M150" s="29"/>
@@ -8891,13 +9134,25 @@
       <c r="R151" s="27"/>
     </row>
     <row r="152" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A152" s="27"/>
-      <c r="B152" s="39"/>
-      <c r="D152" s="31"/>
-      <c r="E152" s="33"/>
+      <c r="A152" s="27" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B152" s="79" t="s">
+        <v>1226</v>
+      </c>
+      <c r="D152" s="31" t="s">
+        <v>312</v>
+      </c>
+      <c r="E152" s="33" t="s">
+        <v>1226</v>
+      </c>
       <c r="G152" s="29"/>
-      <c r="H152" s="31"/>
-      <c r="I152" s="33"/>
+      <c r="H152" s="31" t="s">
+        <v>312</v>
+      </c>
+      <c r="I152" s="33" t="s">
+        <v>1227</v>
+      </c>
       <c r="K152" s="29"/>
       <c r="L152" s="31"/>
       <c r="M152" s="29"/>
@@ -8923,13 +9178,25 @@
       <c r="R153" s="27"/>
     </row>
     <row r="154" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A154" s="27"/>
-      <c r="B154" s="39"/>
-      <c r="D154" s="31"/>
-      <c r="E154" s="33"/>
+      <c r="A154" s="64" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B154" s="80" t="s">
+        <v>1251</v>
+      </c>
+      <c r="D154" s="70" t="s">
+        <v>1250</v>
+      </c>
+      <c r="E154" s="69" t="s">
+        <v>20</v>
+      </c>
       <c r="G154" s="29"/>
-      <c r="H154" s="31"/>
-      <c r="I154" s="33"/>
+      <c r="H154" s="70" t="s">
+        <v>1250</v>
+      </c>
+      <c r="I154" s="69" t="s">
+        <v>1251</v>
+      </c>
       <c r="K154" s="29"/>
       <c r="L154" s="31"/>
       <c r="M154" s="29"/>
@@ -8939,13 +9206,25 @@
       <c r="R154" s="27"/>
     </row>
     <row r="155" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A155" s="27"/>
-      <c r="B155" s="39"/>
-      <c r="D155" s="31"/>
-      <c r="E155" s="33"/>
+      <c r="A155" s="64" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B155" s="80" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D155" s="70" t="s">
+        <v>1252</v>
+      </c>
+      <c r="E155" s="69" t="s">
+        <v>20</v>
+      </c>
       <c r="G155" s="29"/>
-      <c r="H155" s="31"/>
-      <c r="I155" s="33"/>
+      <c r="H155" s="70" t="s">
+        <v>1252</v>
+      </c>
+      <c r="I155" s="69" t="s">
+        <v>1253</v>
+      </c>
       <c r="K155" s="29"/>
       <c r="L155" s="31"/>
       <c r="M155" s="29"/>
@@ -8955,13 +9234,25 @@
       <c r="R155" s="27"/>
     </row>
     <row r="156" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A156" s="27"/>
-      <c r="B156" s="39"/>
-      <c r="D156" s="31"/>
-      <c r="E156" s="33"/>
+      <c r="A156" s="64" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B156" s="80" t="s">
+        <v>1256</v>
+      </c>
+      <c r="D156" s="70" t="s">
+        <v>1254</v>
+      </c>
+      <c r="E156" s="69" t="s">
+        <v>20</v>
+      </c>
       <c r="G156" s="29"/>
-      <c r="H156" s="31"/>
-      <c r="I156" s="33"/>
+      <c r="H156" s="70" t="s">
+        <v>1254</v>
+      </c>
+      <c r="I156" s="69" t="s">
+        <v>1256</v>
+      </c>
       <c r="K156" s="29"/>
       <c r="L156" s="31"/>
       <c r="M156" s="29"/>
@@ -23706,6 +23997,134 @@
       <c r="Q1077" s="32"/>
       <c r="R1077" s="27"/>
     </row>
+    <row r="1078" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1078" s="27"/>
+      <c r="B1078" s="39"/>
+      <c r="D1078" s="31"/>
+      <c r="E1078" s="33"/>
+      <c r="G1078" s="29"/>
+      <c r="H1078" s="31"/>
+      <c r="I1078" s="33"/>
+      <c r="K1078" s="29"/>
+      <c r="L1078" s="31"/>
+      <c r="M1078" s="29"/>
+      <c r="N1078" s="33"/>
+      <c r="P1078" s="29"/>
+      <c r="Q1078" s="32"/>
+      <c r="R1078" s="27"/>
+    </row>
+    <row r="1079" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1079" s="27"/>
+      <c r="B1079" s="39"/>
+      <c r="D1079" s="31"/>
+      <c r="E1079" s="33"/>
+      <c r="G1079" s="29"/>
+      <c r="H1079" s="31"/>
+      <c r="I1079" s="33"/>
+      <c r="K1079" s="29"/>
+      <c r="L1079" s="31"/>
+      <c r="M1079" s="29"/>
+      <c r="N1079" s="33"/>
+      <c r="P1079" s="29"/>
+      <c r="Q1079" s="32"/>
+      <c r="R1079" s="27"/>
+    </row>
+    <row r="1080" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1080" s="27"/>
+      <c r="B1080" s="39"/>
+      <c r="D1080" s="31"/>
+      <c r="E1080" s="33"/>
+      <c r="G1080" s="29"/>
+      <c r="H1080" s="31"/>
+      <c r="I1080" s="33"/>
+      <c r="K1080" s="29"/>
+      <c r="L1080" s="31"/>
+      <c r="M1080" s="29"/>
+      <c r="N1080" s="33"/>
+      <c r="P1080" s="29"/>
+      <c r="Q1080" s="32"/>
+      <c r="R1080" s="27"/>
+    </row>
+    <row r="1081" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1081" s="27"/>
+      <c r="B1081" s="39"/>
+      <c r="D1081" s="31"/>
+      <c r="E1081" s="33"/>
+      <c r="G1081" s="29"/>
+      <c r="H1081" s="31"/>
+      <c r="I1081" s="33"/>
+      <c r="K1081" s="29"/>
+      <c r="L1081" s="31"/>
+      <c r="M1081" s="29"/>
+      <c r="N1081" s="33"/>
+      <c r="P1081" s="29"/>
+      <c r="Q1081" s="32"/>
+      <c r="R1081" s="27"/>
+    </row>
+    <row r="1082" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1082" s="27"/>
+      <c r="B1082" s="39"/>
+      <c r="D1082" s="31"/>
+      <c r="E1082" s="33"/>
+      <c r="G1082" s="29"/>
+      <c r="H1082" s="31"/>
+      <c r="I1082" s="33"/>
+      <c r="K1082" s="29"/>
+      <c r="L1082" s="31"/>
+      <c r="M1082" s="29"/>
+      <c r="N1082" s="33"/>
+      <c r="P1082" s="29"/>
+      <c r="Q1082" s="32"/>
+      <c r="R1082" s="27"/>
+    </row>
+    <row r="1083" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1083" s="27"/>
+      <c r="B1083" s="39"/>
+      <c r="D1083" s="31"/>
+      <c r="E1083" s="33"/>
+      <c r="G1083" s="29"/>
+      <c r="H1083" s="31"/>
+      <c r="I1083" s="33"/>
+      <c r="K1083" s="29"/>
+      <c r="L1083" s="31"/>
+      <c r="M1083" s="29"/>
+      <c r="N1083" s="33"/>
+      <c r="P1083" s="29"/>
+      <c r="Q1083" s="32"/>
+      <c r="R1083" s="27"/>
+    </row>
+    <row r="1084" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1084" s="27"/>
+      <c r="B1084" s="39"/>
+      <c r="D1084" s="31"/>
+      <c r="E1084" s="33"/>
+      <c r="G1084" s="29"/>
+      <c r="H1084" s="31"/>
+      <c r="I1084" s="33"/>
+      <c r="K1084" s="29"/>
+      <c r="L1084" s="31"/>
+      <c r="M1084" s="29"/>
+      <c r="N1084" s="33"/>
+      <c r="P1084" s="29"/>
+      <c r="Q1084" s="32"/>
+      <c r="R1084" s="27"/>
+    </row>
+    <row r="1085" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1085" s="27"/>
+      <c r="B1085" s="39"/>
+      <c r="D1085" s="31"/>
+      <c r="E1085" s="33"/>
+      <c r="G1085" s="29"/>
+      <c r="H1085" s="31"/>
+      <c r="I1085" s="33"/>
+      <c r="K1085" s="29"/>
+      <c r="L1085" s="31"/>
+      <c r="M1085" s="29"/>
+      <c r="N1085" s="33"/>
+      <c r="P1085" s="29"/>
+      <c r="Q1085" s="32"/>
+      <c r="R1085" s="27"/>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -23720,9 +24139,9 @@
   </sheetPr>
   <dimension ref="A1:AB1016"/>
   <sheetViews>
-    <sheetView zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C80" sqref="C80"/>
+      <selection pane="topRight" activeCell="A48" sqref="A48:XFD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -40030,9 +40449,9 @@
   </sheetPr>
   <dimension ref="A1:AB1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D52" sqref="D52"/>
+      <selection pane="topRight" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -59638,8 +60057,8 @@
   </sheetPr>
   <dimension ref="A1:AB1030"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -60974,30 +61393,60 @@
       <c r="Q47" s="32"/>
     </row>
     <row r="48" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B48" s="27"/>
+      <c r="A48" s="81" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B48" s="64" t="s">
+        <v>1270</v>
+      </c>
       <c r="C48" s="32"/>
-      <c r="D48" s="25"/>
+      <c r="D48" s="82" t="s">
+        <v>1269</v>
+      </c>
+      <c r="E48" s="84" t="s">
+        <v>1270</v>
+      </c>
       <c r="F48" s="30"/>
-      <c r="H48" s="30"/>
+      <c r="H48" s="83" t="s">
+        <v>1269</v>
+      </c>
+      <c r="I48" s="84" t="s">
+        <v>1271</v>
+      </c>
       <c r="J48" s="30"/>
       <c r="L48" s="30"/>
       <c r="M48" s="25"/>
       <c r="O48" s="30"/>
       <c r="Q48" s="32"/>
     </row>
-    <row r="49" spans="2:17" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B49" s="27"/>
+    <row r="49" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A49" s="81" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B49" s="64" t="s">
+        <v>1274</v>
+      </c>
       <c r="C49" s="32"/>
-      <c r="D49" s="25"/>
+      <c r="D49" s="82" t="s">
+        <v>1273</v>
+      </c>
+      <c r="E49" s="84" t="s">
+        <v>1274</v>
+      </c>
       <c r="F49" s="30"/>
-      <c r="H49" s="30"/>
+      <c r="H49" s="83" t="s">
+        <v>1273</v>
+      </c>
+      <c r="I49" s="84" t="s">
+        <v>1275</v>
+      </c>
       <c r="J49" s="30"/>
       <c r="L49" s="30"/>
       <c r="M49" s="25"/>
       <c r="O49" s="30"/>
       <c r="Q49" s="32"/>
     </row>
-    <row r="50" spans="2:17" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B50" s="27"/>
       <c r="C50" s="32"/>
       <c r="D50" s="25"/>
@@ -61009,7 +61458,7 @@
       <c r="O50" s="30"/>
       <c r="Q50" s="32"/>
     </row>
-    <row r="51" spans="2:17" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B51" s="27"/>
       <c r="C51" s="32"/>
       <c r="D51" s="25"/>
@@ -61021,7 +61470,7 @@
       <c r="O51" s="30"/>
       <c r="Q51" s="32"/>
     </row>
-    <row r="52" spans="2:17" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B52" s="27"/>
       <c r="C52" s="32"/>
       <c r="D52" s="25"/>
@@ -61033,7 +61482,7 @@
       <c r="O52" s="30"/>
       <c r="Q52" s="32"/>
     </row>
-    <row r="53" spans="2:17" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B53" s="27"/>
       <c r="C53" s="32"/>
       <c r="D53" s="25"/>
@@ -61045,7 +61494,7 @@
       <c r="O53" s="30"/>
       <c r="Q53" s="32"/>
     </row>
-    <row r="54" spans="2:17" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B54" s="27"/>
       <c r="C54" s="32"/>
       <c r="D54" s="25"/>
@@ -61057,7 +61506,7 @@
       <c r="O54" s="30"/>
       <c r="Q54" s="32"/>
     </row>
-    <row r="55" spans="2:17" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B55" s="27"/>
       <c r="C55" s="32"/>
       <c r="D55" s="25"/>
@@ -61069,7 +61518,7 @@
       <c r="O55" s="30"/>
       <c r="Q55" s="32"/>
     </row>
-    <row r="56" spans="2:17" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B56" s="27"/>
       <c r="C56" s="32"/>
       <c r="D56" s="25"/>
@@ -61081,7 +61530,7 @@
       <c r="O56" s="30"/>
       <c r="Q56" s="32"/>
     </row>
-    <row r="57" spans="2:17" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B57" s="27"/>
       <c r="C57" s="32"/>
       <c r="D57" s="25"/>
@@ -61093,7 +61542,7 @@
       <c r="O57" s="30"/>
       <c r="Q57" s="32"/>
     </row>
-    <row r="58" spans="2:17" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B58" s="27"/>
       <c r="C58" s="32"/>
       <c r="D58" s="25"/>
@@ -61105,7 +61554,7 @@
       <c r="O58" s="30"/>
       <c r="Q58" s="32"/>
     </row>
-    <row r="59" spans="2:17" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B59" s="27"/>
       <c r="C59" s="32"/>
       <c r="D59" s="25"/>
@@ -61117,7 +61566,7 @@
       <c r="O59" s="30"/>
       <c r="Q59" s="32"/>
     </row>
-    <row r="60" spans="2:17" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B60" s="27"/>
       <c r="C60" s="32"/>
       <c r="D60" s="25"/>
@@ -61129,7 +61578,7 @@
       <c r="O60" s="30"/>
       <c r="Q60" s="32"/>
     </row>
-    <row r="61" spans="2:17" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B61" s="27"/>
       <c r="C61" s="32"/>
       <c r="D61" s="25"/>
@@ -61141,7 +61590,7 @@
       <c r="O61" s="30"/>
       <c r="Q61" s="32"/>
     </row>
-    <row r="62" spans="2:17" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B62" s="27"/>
       <c r="C62" s="32"/>
       <c r="D62" s="25"/>
@@ -61153,7 +61602,7 @@
       <c r="O62" s="30"/>
       <c r="Q62" s="32"/>
     </row>
-    <row r="63" spans="2:17" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B63" s="27"/>
       <c r="C63" s="32"/>
       <c r="D63" s="25"/>
@@ -61165,7 +61614,7 @@
       <c r="O63" s="30"/>
       <c r="Q63" s="32"/>
     </row>
-    <row r="64" spans="2:17" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B64" s="27"/>
       <c r="C64" s="32"/>
       <c r="D64" s="25"/>

</xml_diff>